<commit_message>
Update investment cost and cap2act in SubRes_RSD.xlsx and filled values in SubRes_RSD_Trans.xlsx
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\main\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AA1899-A6F1-4A4A-AB6F-A5983C6A2293}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F9EB5-C743-485E-8A18-87836CAB3D61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="2715" windowWidth="14400" windowHeight="6795" tabRatio="819" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37" yWindow="14385" windowWidth="14401" windowHeight="6795" tabRatio="819" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>
@@ -1741,7 +1741,7 @@
                   <a14:compatExt spid="_x0000_s89089"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000015C0100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000015C0100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5153,7 +5153,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="32" t="str">
-        <f t="shared" ref="B6:B18" si="0">"R-S*"&amp;F6&amp;"_"&amp;G6&amp;"*"</f>
+        <f t="shared" ref="B6:B16" si="0">"R-S*"&amp;F6&amp;"_"&amp;G6&amp;"*"</f>
         <v>R-S*Apt_COA*</v>
       </c>
       <c r="C6" s="32" t="str">
@@ -5548,7 +5548,7 @@
       </c>
       <c r="D17" s="33">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H17,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>5.0677847327291303E-2</v>
+        <v>5.3179934471147799E-2</v>
       </c>
       <c r="F17" s="33" t="s">
         <v>109</v>
@@ -5648,7 +5648,7 @@
         <v>82</v>
       </c>
       <c r="H20" s="32" t="str">
-        <f t="shared" ref="H20:H25" si="6">"R-S*_"&amp;F20&amp;"_"&amp;G20&amp;"*"</f>
+        <f t="shared" ref="H20:H23" si="6">"R-S*_"&amp;F20&amp;"_"&amp;G20&amp;"*"</f>
         <v>R-S*_Att_COA*</v>
       </c>
       <c r="J20" s="32" t="s">
@@ -5823,7 +5823,7 @@
         <v>201</v>
       </c>
       <c r="H25" s="33" t="str">
-        <f t="shared" ref="H25:H30" si="7">"R-S*_"&amp;F25&amp;"_"&amp;G25&amp;"*"</f>
+        <f t="shared" ref="H25" si="7">"R-S*_"&amp;F25&amp;"_"&amp;G25&amp;"*"</f>
         <v>R-S*_Att_KER*</v>
       </c>
     </row>
@@ -5976,7 +5976,7 @@
       </c>
       <c r="D31" s="33">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H31,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.23960518419681501</v>
+        <v>0.249048421589953</v>
       </c>
       <c r="F31" s="33" t="s">
         <v>105</v>
@@ -6051,7 +6051,7 @@
         <v>82</v>
       </c>
       <c r="H34" s="32" t="str">
-        <f t="shared" ref="H34:H39" si="10">"R-S*_"&amp;F34&amp;"_"&amp;G34&amp;"*"</f>
+        <f t="shared" ref="H34:H37" si="10">"R-S*_"&amp;F34&amp;"_"&amp;G34&amp;"*"</f>
         <v>R-S*_Det_COA*</v>
       </c>
       <c r="I34" s="25"/>
@@ -6187,7 +6187,7 @@
         <v>201</v>
       </c>
       <c r="H39" s="33" t="str">
-        <f t="shared" ref="H39:H44" si="11">"R-S*_"&amp;F39&amp;"_"&amp;G39&amp;"*"</f>
+        <f t="shared" ref="H39" si="11">"R-S*_"&amp;F39&amp;"_"&amp;G39&amp;"*"</f>
         <v>R-S*_Det_KER*</v>
       </c>
     </row>
@@ -6340,7 +6340,7 @@
       </c>
       <c r="D45" s="33">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H45,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.21841678709847501</v>
+        <v>0.22978380047467101</v>
       </c>
       <c r="F45" s="33" t="s">
         <v>115</v>
@@ -6579,7 +6579,7 @@
         <v>110</v>
       </c>
       <c r="H55" s="33" t="str">
-        <f>"R-WH_"&amp;F55&amp;"_"&amp;G55&amp;"*"</f>
+        <f t="shared" ref="H55:H60" si="14">"R-WH_"&amp;F55&amp;"_"&amp;G55&amp;"*"</f>
         <v>R-WH_Apt_PEA*</v>
       </c>
     </row>
@@ -6603,7 +6603,7 @@
         <v>111</v>
       </c>
       <c r="H56" s="32" t="str">
-        <f>"R-WH_"&amp;F56&amp;"_"&amp;G56&amp;"*"</f>
+        <f t="shared" si="14"/>
         <v>R-WH_Apt_SMF*</v>
       </c>
     </row>
@@ -6627,7 +6627,7 @@
         <v>203</v>
       </c>
       <c r="H57" s="33" t="str">
-        <f>"R-WH_"&amp;F57&amp;"_"&amp;G57&amp;"*"</f>
+        <f t="shared" si="14"/>
         <v>R-WH_Apt_WOO*</v>
       </c>
     </row>
@@ -6651,7 +6651,7 @@
         <v>84</v>
       </c>
       <c r="H58" s="32" t="str">
-        <f>"R-WH_"&amp;F58&amp;"_"&amp;G58&amp;"*"</f>
+        <f t="shared" si="14"/>
         <v>R-WH_Apt_HET*</v>
       </c>
     </row>
@@ -6675,7 +6675,7 @@
         <v>204</v>
       </c>
       <c r="H59" s="33" t="str">
-        <f>"R-WH_"&amp;F59&amp;"_"&amp;G59&amp;"*"</f>
+        <f t="shared" si="14"/>
         <v>R-WH_Apt_GEO*</v>
       </c>
     </row>
@@ -6699,7 +6699,7 @@
         <v>250</v>
       </c>
       <c r="H60" s="32" t="str">
-        <f>"R-WH_"&amp;F60&amp;"_"&amp;G60&amp;"*"</f>
+        <f t="shared" si="14"/>
         <v>R-WH_Apt_SOL*</v>
       </c>
     </row>
@@ -6720,7 +6720,7 @@
         <v>1</v>
       </c>
       <c r="B62" s="32" t="str">
-        <f t="shared" ref="B62:B73" si="14">"R-WH_"&amp;F62&amp;"_"&amp;G62&amp;"*"</f>
+        <f t="shared" ref="B62:B73" si="15">"R-WH_"&amp;F62&amp;"_"&amp;G62&amp;"*"</f>
         <v>R-WH_Att_COA*</v>
       </c>
       <c r="C62" s="32"/>
@@ -6735,7 +6735,7 @@
         <v>82</v>
       </c>
       <c r="H62" s="32" t="str">
-        <f t="shared" ref="H62:H67" si="15">"R-WH_"&amp;F62&amp;"_"&amp;G62&amp;"*"</f>
+        <f t="shared" ref="H62:H67" si="16">"R-WH_"&amp;F62&amp;"_"&amp;G62&amp;"*"</f>
         <v>R-WH_Att_COA*</v>
       </c>
     </row>
@@ -6744,7 +6744,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_BDL*</v>
       </c>
       <c r="C63" s="33"/>
@@ -6759,7 +6759,7 @@
         <v>199</v>
       </c>
       <c r="H63" s="33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>R-WH_Att_BDL*</v>
       </c>
     </row>
@@ -6768,7 +6768,7 @@
         <v>1</v>
       </c>
       <c r="B64" s="32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_ETH*</v>
       </c>
       <c r="C64" s="32"/>
@@ -6783,7 +6783,7 @@
         <v>198</v>
       </c>
       <c r="H64" s="32" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>R-WH_Att_ETH*</v>
       </c>
     </row>
@@ -6792,7 +6792,7 @@
         <v>263</v>
       </c>
       <c r="B65" s="33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_LPG*</v>
       </c>
       <c r="C65" s="33"/>
@@ -6807,7 +6807,7 @@
         <v>200</v>
       </c>
       <c r="H65" s="33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>R-WH_Att_LPG*</v>
       </c>
     </row>
@@ -6816,7 +6816,7 @@
         <v>263</v>
       </c>
       <c r="B66" s="32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_ELC*</v>
       </c>
       <c r="C66" s="32"/>
@@ -6840,7 +6840,7 @@
         <v>1</v>
       </c>
       <c r="B67" s="33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_KER*</v>
       </c>
       <c r="C67" s="33"/>
@@ -6855,7 +6855,7 @@
         <v>201</v>
       </c>
       <c r="H67" s="33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>R-WH_Att_KER*</v>
       </c>
     </row>
@@ -6864,7 +6864,7 @@
         <v>263</v>
       </c>
       <c r="B68" s="32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_GAS*</v>
       </c>
       <c r="C68" s="32"/>
@@ -6888,7 +6888,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_PEA*</v>
       </c>
       <c r="C69" s="33"/>
@@ -6903,7 +6903,7 @@
         <v>110</v>
       </c>
       <c r="H69" s="33" t="str">
-        <f>"R-WH_"&amp;F69&amp;"_"&amp;G69&amp;"*"</f>
+        <f t="shared" ref="H69:H74" si="17">"R-WH_"&amp;F69&amp;"_"&amp;G69&amp;"*"</f>
         <v>R-WH_Att_PEA*</v>
       </c>
     </row>
@@ -6912,7 +6912,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_SMF*</v>
       </c>
       <c r="C70" s="32"/>
@@ -6927,7 +6927,7 @@
         <v>111</v>
       </c>
       <c r="H70" s="32" t="str">
-        <f>"R-WH_"&amp;F70&amp;"_"&amp;G70&amp;"*"</f>
+        <f t="shared" si="17"/>
         <v>R-WH_Att_SMF*</v>
       </c>
     </row>
@@ -6936,7 +6936,7 @@
         <v>263</v>
       </c>
       <c r="B71" s="33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_WOO*</v>
       </c>
       <c r="C71" s="33"/>
@@ -6951,7 +6951,7 @@
         <v>203</v>
       </c>
       <c r="H71" s="33" t="str">
-        <f>"R-WH_"&amp;F71&amp;"_"&amp;G71&amp;"*"</f>
+        <f t="shared" si="17"/>
         <v>R-WH_Att_WOO*</v>
       </c>
     </row>
@@ -6960,7 +6960,7 @@
         <v>1</v>
       </c>
       <c r="B72" s="32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_HET*</v>
       </c>
       <c r="C72" s="32"/>
@@ -6975,7 +6975,7 @@
         <v>84</v>
       </c>
       <c r="H72" s="32" t="str">
-        <f>"R-WH_"&amp;F72&amp;"_"&amp;G72&amp;"*"</f>
+        <f t="shared" si="17"/>
         <v>R-WH_Att_HET*</v>
       </c>
     </row>
@@ -6984,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="B73" s="33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-WH_Att_GEO*</v>
       </c>
       <c r="C73" s="33"/>
@@ -6999,7 +6999,7 @@
         <v>204</v>
       </c>
       <c r="H73" s="33" t="str">
-        <f>"R-WH_"&amp;F73&amp;"_"&amp;G73&amp;"*"</f>
+        <f t="shared" si="17"/>
         <v>R-WH_Att_GEO*</v>
       </c>
     </row>
@@ -7023,7 +7023,7 @@
         <v>250</v>
       </c>
       <c r="H74" s="32" t="str">
-        <f>"R-WH_"&amp;F74&amp;"_"&amp;G74&amp;"*"</f>
+        <f t="shared" si="17"/>
         <v>R-WH_Att_SOL*</v>
       </c>
     </row>
@@ -7044,7 +7044,7 @@
         <v>1</v>
       </c>
       <c r="B76" s="32" t="str">
-        <f t="shared" ref="B76:B87" si="16">"R-WH_"&amp;F76&amp;"_"&amp;G76&amp;"*"</f>
+        <f t="shared" ref="B76:B87" si="18">"R-WH_"&amp;F76&amp;"_"&amp;G76&amp;"*"</f>
         <v>R-WH_Det_COA*</v>
       </c>
       <c r="C76" s="32"/>
@@ -7059,7 +7059,7 @@
         <v>82</v>
       </c>
       <c r="H76" s="32" t="str">
-        <f t="shared" ref="H76:H81" si="17">"R-WH_"&amp;F76&amp;"_"&amp;G76&amp;"*"</f>
+        <f t="shared" ref="H76:H81" si="19">"R-WH_"&amp;F76&amp;"_"&amp;G76&amp;"*"</f>
         <v>R-WH_Det_COA*</v>
       </c>
     </row>
@@ -7068,7 +7068,7 @@
         <v>1</v>
       </c>
       <c r="B77" s="33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_BDL*</v>
       </c>
       <c r="C77" s="33"/>
@@ -7083,7 +7083,7 @@
         <v>199</v>
       </c>
       <c r="H77" s="33" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>R-WH_Det_BDL*</v>
       </c>
     </row>
@@ -7092,7 +7092,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_ETH*</v>
       </c>
       <c r="C78" s="32"/>
@@ -7107,7 +7107,7 @@
         <v>198</v>
       </c>
       <c r="H78" s="32" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>R-WH_Det_ETH*</v>
       </c>
     </row>
@@ -7116,7 +7116,7 @@
         <v>263</v>
       </c>
       <c r="B79" s="33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_LPG*</v>
       </c>
       <c r="C79" s="33"/>
@@ -7131,7 +7131,7 @@
         <v>200</v>
       </c>
       <c r="H79" s="33" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>R-WH_Det_LPG*</v>
       </c>
     </row>
@@ -7140,7 +7140,7 @@
         <v>263</v>
       </c>
       <c r="B80" s="32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_ELC*</v>
       </c>
       <c r="C80" s="32"/>
@@ -7164,7 +7164,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_KER*</v>
       </c>
       <c r="C81" s="33"/>
@@ -7179,7 +7179,7 @@
         <v>201</v>
       </c>
       <c r="H81" s="33" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>R-WH_Det_KER*</v>
       </c>
     </row>
@@ -7188,7 +7188,7 @@
         <v>263</v>
       </c>
       <c r="B82" s="32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_GAS*</v>
       </c>
       <c r="C82" s="32"/>
@@ -7212,7 +7212,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_PEA*</v>
       </c>
       <c r="C83" s="33"/>
@@ -7227,7 +7227,7 @@
         <v>110</v>
       </c>
       <c r="H83" s="33" t="str">
-        <f>"R-WH_"&amp;F83&amp;"_"&amp;G83&amp;"*"</f>
+        <f t="shared" ref="H83:H88" si="20">"R-WH_"&amp;F83&amp;"_"&amp;G83&amp;"*"</f>
         <v>R-WH_Det_PEA*</v>
       </c>
     </row>
@@ -7236,7 +7236,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_SMF*</v>
       </c>
       <c r="C84" s="32"/>
@@ -7251,7 +7251,7 @@
         <v>111</v>
       </c>
       <c r="H84" s="32" t="str">
-        <f>"R-WH_"&amp;F84&amp;"_"&amp;G84&amp;"*"</f>
+        <f t="shared" si="20"/>
         <v>R-WH_Det_SMF*</v>
       </c>
     </row>
@@ -7260,7 +7260,7 @@
         <v>263</v>
       </c>
       <c r="B85" s="33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_WOO*</v>
       </c>
       <c r="C85" s="33"/>
@@ -7275,7 +7275,7 @@
         <v>203</v>
       </c>
       <c r="H85" s="33" t="str">
-        <f>"R-WH_"&amp;F85&amp;"_"&amp;G85&amp;"*"</f>
+        <f t="shared" si="20"/>
         <v>R-WH_Det_WOO*</v>
       </c>
     </row>
@@ -7284,7 +7284,7 @@
         <v>1</v>
       </c>
       <c r="B86" s="32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_HET*</v>
       </c>
       <c r="C86" s="32"/>
@@ -7299,7 +7299,7 @@
         <v>84</v>
       </c>
       <c r="H86" s="32" t="str">
-        <f>"R-WH_"&amp;F86&amp;"_"&amp;G86&amp;"*"</f>
+        <f t="shared" si="20"/>
         <v>R-WH_Det_HET*</v>
       </c>
     </row>
@@ -7308,7 +7308,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>R-WH_Det_GEO*</v>
       </c>
       <c r="C87" s="33"/>
@@ -7323,7 +7323,7 @@
         <v>204</v>
       </c>
       <c r="H87" s="33" t="str">
-        <f>"R-WH_"&amp;F87&amp;"_"&amp;G87&amp;"*"</f>
+        <f t="shared" si="20"/>
         <v>R-WH_Det_GEO*</v>
       </c>
     </row>
@@ -7347,7 +7347,7 @@
         <v>250</v>
       </c>
       <c r="H88" s="32" t="str">
-        <f>"R-WH_"&amp;F88&amp;"_"&amp;G88&amp;"*"</f>
+        <f t="shared" si="20"/>
         <v>R-WH_Det_SOL*</v>
       </c>
     </row>
@@ -7385,7 +7385,7 @@
         <v>82</v>
       </c>
       <c r="H90" s="32" t="str">
-        <f t="shared" ref="H90:H93" si="18">"R-WH_"&amp;F90&amp;"_"&amp;G90&amp;"*"</f>
+        <f t="shared" ref="H90:H93" si="21">"R-WH_"&amp;F90&amp;"_"&amp;G90&amp;"*"</f>
         <v>R-WH_Apt_COA*</v>
       </c>
     </row>
@@ -7394,11 +7394,11 @@
         <v>1</v>
       </c>
       <c r="B91" s="33" t="str">
-        <f t="shared" ref="B91:B102" si="19">"R-SW_"&amp;F91&amp;"_"&amp;G91&amp;"*"</f>
+        <f t="shared" ref="B91:B102" si="22">"R-SW_"&amp;F91&amp;"_"&amp;G91&amp;"*"</f>
         <v>R-SW_Apt_BDL*</v>
       </c>
       <c r="C91" s="33" t="str">
-        <f t="shared" ref="C91:C102" si="20">"RSDWH_"&amp;F91</f>
+        <f t="shared" ref="C91:C102" si="23">"RSDWH_"&amp;F91</f>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D91" s="33">
@@ -7412,7 +7412,7 @@
         <v>199</v>
       </c>
       <c r="H91" s="33" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>R-WH_Apt_BDL*</v>
       </c>
     </row>
@@ -7421,11 +7421,11 @@
         <v>1</v>
       </c>
       <c r="B92" s="32" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_ETH*</v>
       </c>
       <c r="C92" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D92" s="32">
@@ -7439,7 +7439,7 @@
         <v>198</v>
       </c>
       <c r="H92" s="32" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>R-WH_Apt_ETH*</v>
       </c>
     </row>
@@ -7448,11 +7448,11 @@
         <v>265</v>
       </c>
       <c r="B93" s="33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_LPG*</v>
       </c>
       <c r="C93" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D93" s="33">
@@ -7466,7 +7466,7 @@
         <v>200</v>
       </c>
       <c r="H93" s="33" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>R-WH_Apt_LPG*</v>
       </c>
     </row>
@@ -7479,7 +7479,7 @@
         <v>R-SW_Apt_ELC_N1</v>
       </c>
       <c r="C94" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D94" s="32">
@@ -7506,7 +7506,7 @@
         <v>R-SW_Apt_ELC_HP*</v>
       </c>
       <c r="C95" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D95" s="32">
@@ -7529,11 +7529,11 @@
         <v>265</v>
       </c>
       <c r="B96" s="33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_KER*</v>
       </c>
       <c r="C96" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D96" s="33">
@@ -7547,7 +7547,7 @@
         <v>201</v>
       </c>
       <c r="H96" s="33" t="str">
-        <f t="shared" ref="H96" si="21">"R-WH_"&amp;F96&amp;"_"&amp;G96&amp;"*"</f>
+        <f t="shared" ref="H96" si="24">"R-WH_"&amp;F96&amp;"_"&amp;G96&amp;"*"</f>
         <v>R-WH_Apt_KER*</v>
       </c>
     </row>
@@ -7556,11 +7556,11 @@
         <v>265</v>
       </c>
       <c r="B97" s="32" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_GAS*</v>
       </c>
       <c r="C97" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D97" s="32">
@@ -7583,11 +7583,11 @@
         <v>1</v>
       </c>
       <c r="B98" s="33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_PEA*</v>
       </c>
       <c r="C98" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D98" s="33">
@@ -7610,11 +7610,11 @@
         <v>1</v>
       </c>
       <c r="B99" s="32" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_SMF*</v>
       </c>
       <c r="C99" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D99" s="32">
@@ -7637,11 +7637,11 @@
         <v>265</v>
       </c>
       <c r="B100" s="33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_WOO*</v>
       </c>
       <c r="C100" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D100" s="33">
@@ -7664,11 +7664,11 @@
         <v>265</v>
       </c>
       <c r="B101" s="32" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_HET*</v>
       </c>
       <c r="C101" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D101" s="32">
@@ -7691,11 +7691,11 @@
         <v>1</v>
       </c>
       <c r="B102" s="33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>R-SW_Apt_SOL*</v>
       </c>
       <c r="C102" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>RSDWH_Apt</v>
       </c>
       <c r="D102" s="33">
@@ -7734,7 +7734,7 @@
         <v>R-SW_Att_COA*</v>
       </c>
       <c r="C104" s="32" t="str">
-        <f t="shared" ref="C104:C116" si="22">"RSDWH_"&amp;F104</f>
+        <f t="shared" ref="C104:C116" si="25">"RSDWH_"&amp;F104</f>
         <v>RSDWH_Att</v>
       </c>
       <c r="D104" s="32">
@@ -7748,7 +7748,7 @@
         <v>82</v>
       </c>
       <c r="H104" s="32" t="str">
-        <f t="shared" ref="H104:H107" si="23">"R-WH_"&amp;F104&amp;"_"&amp;G104&amp;"*"</f>
+        <f t="shared" ref="H104:H107" si="26">"R-WH_"&amp;F104&amp;"_"&amp;G104&amp;"*"</f>
         <v>R-WH_Att_COA*</v>
       </c>
     </row>
@@ -7757,11 +7757,11 @@
         <v>1</v>
       </c>
       <c r="B105" s="33" t="str">
-        <f t="shared" ref="B105:B116" si="24">"R-SW_"&amp;F105&amp;"_"&amp;G105&amp;"*"</f>
+        <f t="shared" ref="B105:B116" si="27">"R-SW_"&amp;F105&amp;"_"&amp;G105&amp;"*"</f>
         <v>R-SW_Att_BDL*</v>
       </c>
       <c r="C105" s="33" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D105" s="33">
@@ -7775,7 +7775,7 @@
         <v>199</v>
       </c>
       <c r="H105" s="33" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-WH_Att_BDL*</v>
       </c>
     </row>
@@ -7784,11 +7784,11 @@
         <v>1</v>
       </c>
       <c r="B106" s="32" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_ETH*</v>
       </c>
       <c r="C106" s="32" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D106" s="32">
@@ -7802,7 +7802,7 @@
         <v>198</v>
       </c>
       <c r="H106" s="32" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-WH_Att_ETH*</v>
       </c>
     </row>
@@ -7811,11 +7811,11 @@
         <v>265</v>
       </c>
       <c r="B107" s="33" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_LPG*</v>
       </c>
       <c r="C107" s="33" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D107" s="33">
@@ -7829,7 +7829,7 @@
         <v>200</v>
       </c>
       <c r="H107" s="33" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-WH_Att_LPG*</v>
       </c>
     </row>
@@ -7842,7 +7842,7 @@
         <v>R-SW_Att_ELC_N1</v>
       </c>
       <c r="C108" s="32" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D108" s="32">
@@ -7869,7 +7869,7 @@
         <v>R-SW_Att_ELC_HP*</v>
       </c>
       <c r="C109" s="32" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D109" s="32">
@@ -7892,11 +7892,11 @@
         <v>265</v>
       </c>
       <c r="B110" s="33" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_KER*</v>
       </c>
       <c r="C110" s="33" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D110" s="33">
@@ -7910,7 +7910,7 @@
         <v>201</v>
       </c>
       <c r="H110" s="33" t="str">
-        <f t="shared" ref="H110" si="25">"R-WH_"&amp;F110&amp;"_"&amp;G110&amp;"*"</f>
+        <f t="shared" ref="H110" si="28">"R-WH_"&amp;F110&amp;"_"&amp;G110&amp;"*"</f>
         <v>R-WH_Att_KER*</v>
       </c>
     </row>
@@ -7919,11 +7919,11 @@
         <v>265</v>
       </c>
       <c r="B111" s="32" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_GAS*</v>
       </c>
       <c r="C111" s="32" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D111" s="32">
@@ -7946,11 +7946,11 @@
         <v>1</v>
       </c>
       <c r="B112" s="33" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_PEA*</v>
       </c>
       <c r="C112" s="33" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D112" s="33">
@@ -7973,11 +7973,11 @@
         <v>1</v>
       </c>
       <c r="B113" s="32" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_SMF*</v>
       </c>
       <c r="C113" s="32" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D113" s="32">
@@ -8000,11 +8000,11 @@
         <v>265</v>
       </c>
       <c r="B114" s="33" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_WOO*</v>
       </c>
       <c r="C114" s="33" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D114" s="33">
@@ -8027,11 +8027,11 @@
         <v>265</v>
       </c>
       <c r="B115" s="32" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_HET*</v>
       </c>
       <c r="C115" s="32" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D115" s="32">
@@ -8054,11 +8054,11 @@
         <v>1</v>
       </c>
       <c r="B116" s="33" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>R-SW_Att_SOL*</v>
       </c>
       <c r="C116" s="33" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>RSDWH_Att</v>
       </c>
       <c r="D116" s="33">
@@ -8093,11 +8093,11 @@
         <v>1</v>
       </c>
       <c r="B118" s="32" t="str">
-        <f t="shared" ref="B118:B130" si="26">"R-SW_"&amp;F118&amp;"_"&amp;G118&amp;"*"</f>
+        <f t="shared" ref="B118:B130" si="29">"R-SW_"&amp;F118&amp;"_"&amp;G118&amp;"*"</f>
         <v>R-SW_Det_COA*</v>
       </c>
       <c r="C118" s="32" t="str">
-        <f t="shared" ref="C118:C130" si="27">"RSDWH_"&amp;F118</f>
+        <f t="shared" ref="C118:C130" si="30">"RSDWH_"&amp;F118</f>
         <v>RSDWH_Det</v>
       </c>
       <c r="D118" s="32">
@@ -8111,7 +8111,7 @@
         <v>82</v>
       </c>
       <c r="H118" s="32" t="str">
-        <f t="shared" ref="H118:H121" si="28">"R-WH_"&amp;F118&amp;"_"&amp;G118&amp;"*"</f>
+        <f t="shared" ref="H118:H121" si="31">"R-WH_"&amp;F118&amp;"_"&amp;G118&amp;"*"</f>
         <v>R-WH_Det_COA*</v>
       </c>
     </row>
@@ -8120,11 +8120,11 @@
         <v>1</v>
       </c>
       <c r="B119" s="33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_BDL*</v>
       </c>
       <c r="C119" s="33" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D119" s="33">
@@ -8138,7 +8138,7 @@
         <v>199</v>
       </c>
       <c r="H119" s="33" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>R-WH_Det_BDL*</v>
       </c>
     </row>
@@ -8147,11 +8147,11 @@
         <v>1</v>
       </c>
       <c r="B120" s="32" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_ETH*</v>
       </c>
       <c r="C120" s="32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D120" s="32">
@@ -8165,7 +8165,7 @@
         <v>198</v>
       </c>
       <c r="H120" s="32" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>R-WH_Det_ETH*</v>
       </c>
     </row>
@@ -8174,11 +8174,11 @@
         <v>265</v>
       </c>
       <c r="B121" s="33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_LPG*</v>
       </c>
       <c r="C121" s="33" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D121" s="33">
@@ -8192,7 +8192,7 @@
         <v>200</v>
       </c>
       <c r="H121" s="33" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>R-WH_Det_LPG*</v>
       </c>
     </row>
@@ -8205,7 +8205,7 @@
         <v>R-SW_Det_ELC_N1</v>
       </c>
       <c r="C122" s="32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D122" s="32">
@@ -8232,7 +8232,7 @@
         <v>R-SW_Det_ELC_HP*</v>
       </c>
       <c r="C123" s="32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D123" s="32">
@@ -8255,11 +8255,11 @@
         <v>265</v>
       </c>
       <c r="B124" s="33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_KER*</v>
       </c>
       <c r="C124" s="33" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D124" s="33">
@@ -8273,7 +8273,7 @@
         <v>201</v>
       </c>
       <c r="H124" s="33" t="str">
-        <f t="shared" ref="H124" si="29">"R-WH_"&amp;F124&amp;"_"&amp;G124&amp;"*"</f>
+        <f t="shared" ref="H124" si="32">"R-WH_"&amp;F124&amp;"_"&amp;G124&amp;"*"</f>
         <v>R-WH_Det_KER*</v>
       </c>
     </row>
@@ -8282,11 +8282,11 @@
         <v>265</v>
       </c>
       <c r="B125" s="32" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_GAS*</v>
       </c>
       <c r="C125" s="32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D125" s="32">
@@ -8309,11 +8309,11 @@
         <v>1</v>
       </c>
       <c r="B126" s="33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_PEA*</v>
       </c>
       <c r="C126" s="33" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D126" s="33">
@@ -8336,11 +8336,11 @@
         <v>1</v>
       </c>
       <c r="B127" s="32" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_SMF*</v>
       </c>
       <c r="C127" s="32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D127" s="32">
@@ -8363,11 +8363,11 @@
         <v>265</v>
       </c>
       <c r="B128" s="33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_WOO*</v>
       </c>
       <c r="C128" s="33" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D128" s="33">
@@ -8390,11 +8390,11 @@
         <v>265</v>
       </c>
       <c r="B129" s="32" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_HET*</v>
       </c>
       <c r="C129" s="32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D129" s="32">
@@ -8417,11 +8417,11 @@
         <v>1</v>
       </c>
       <c r="B130" s="38" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Det_SOL*</v>
       </c>
       <c r="C130" s="38" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>RSDWH_Det</v>
       </c>
       <c r="D130" s="38">
@@ -8471,7 +8471,7 @@
         <v>83</v>
       </c>
       <c r="H132" s="39" t="str">
-        <f t="shared" ref="H132:H134" si="30">"R-SH_"&amp;F132&amp;"_"&amp;G132&amp;"*X1"</f>
+        <f t="shared" ref="H132:H134" si="33">"R-SH_"&amp;F132&amp;"_"&amp;G132&amp;"*X1"</f>
         <v>R-SH_Apt_ELC*X1</v>
       </c>
     </row>
@@ -8495,7 +8495,7 @@
         <v>83</v>
       </c>
       <c r="H133" s="39" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
@@ -8519,7 +8519,7 @@
         <v>83</v>
       </c>
       <c r="H134" s="39" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
     </row>
@@ -8558,7 +8558,7 @@
         <v>83</v>
       </c>
       <c r="H136" s="39" t="str">
-        <f t="shared" ref="H136:H138" si="31">"R-SH_"&amp;F136&amp;"_"&amp;G136&amp;"*X1"</f>
+        <f t="shared" ref="H136:H138" si="34">"R-SH_"&amp;F136&amp;"_"&amp;G136&amp;"*X1"</f>
         <v>R-SH_Apt_ELC*X1</v>
       </c>
     </row>
@@ -8585,7 +8585,7 @@
         <v>83</v>
       </c>
       <c r="H137" s="39" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
@@ -8612,7 +8612,7 @@
         <v>83</v>
       </c>
       <c r="H138" s="41" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
     </row>
@@ -12608,10 +12608,10 @@
         <v>132</v>
       </c>
       <c r="L8">
-        <v>5.0677847327291303E-2</v>
+        <v>5.3179934471147799E-2</v>
       </c>
       <c r="M8">
-        <v>5.0677847327291303E-2</v>
+        <v>5.3179934471147799E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -13141,10 +13141,10 @@
         <v>132</v>
       </c>
       <c r="L21">
-        <v>0.23960518419681501</v>
+        <v>0.249048421589953</v>
       </c>
       <c r="M21">
-        <v>0.23960518419681501</v>
+        <v>0.249048421589953</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -13674,10 +13674,10 @@
         <v>132</v>
       </c>
       <c r="L34">
-        <v>0.21841678709847501</v>
+        <v>0.22978380047467101</v>
       </c>
       <c r="M34">
-        <v>0.21841678709847501</v>
+        <v>0.22978380047467101</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Disable updating of not available GAS, LPG and WOOD water heating
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\main\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC51D45-C114-4D77-A88D-18108CC5BFF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE0E4E0-8581-4111-8673-4E1BF79BE6E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1230" windowWidth="28800" windowHeight="7800" tabRatio="819" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>
@@ -5063,8 +5063,8 @@
   </sheetPr>
   <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6465,7 +6465,7 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B51" s="33" t="str">
         <f t="shared" si="12"/>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B54" s="32" t="str">
         <f t="shared" si="12"/>
@@ -6609,7 +6609,7 @@
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B57" s="33" t="str">
         <f t="shared" si="12"/>
@@ -6789,7 +6789,7 @@
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B65" s="33" t="str">
         <f t="shared" si="15"/>
@@ -6861,7 +6861,7 @@
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B68" s="32" t="str">
         <f t="shared" si="15"/>
@@ -6933,7 +6933,7 @@
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B71" s="33" t="str">
         <f t="shared" si="15"/>
@@ -7113,7 +7113,7 @@
     </row>
     <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B79" s="33" t="str">
         <f t="shared" si="18"/>
@@ -7185,7 +7185,7 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="32" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B82" s="32" t="str">
         <f t="shared" si="18"/>
@@ -7257,7 +7257,7 @@
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B85" s="33" t="str">
         <f t="shared" si="18"/>
@@ -8629,8 +8629,8 @@
   </sheetPr>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9778,7 +9778,7 @@
         <v>R-WH_Apt_LPG*</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F55" s="33" t="str">
         <f t="shared" si="4"/>
@@ -9870,7 +9870,7 @@
         <v>R-WH_Apt_GAS*</v>
       </c>
       <c r="E59" s="32" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F59" s="32" t="str">
         <f t="shared" si="4"/>
@@ -9939,7 +9939,7 @@
         <v>R-WH_Apt_WOO*</v>
       </c>
       <c r="E62" s="33" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F62" s="33" t="str">
         <f t="shared" si="4"/>
@@ -10087,7 +10087,7 @@
         <v>R-WH_Att_LPG*</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F69" s="33" t="str">
         <f t="shared" si="6"/>
@@ -10179,7 +10179,7 @@
         <v>R-WH_Att_GAS*</v>
       </c>
       <c r="E73" s="32" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F73" s="32" t="str">
         <f t="shared" si="6"/>
@@ -10248,7 +10248,7 @@
         <v>R-WH_Att_WOO*</v>
       </c>
       <c r="E76" s="33" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F76" s="33" t="str">
         <f t="shared" si="6"/>
@@ -10396,7 +10396,7 @@
         <v>R-WH_Det_LPG*</v>
       </c>
       <c r="E83" s="33" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F83" s="33" t="str">
         <f t="shared" si="9"/>
@@ -10488,7 +10488,7 @@
         <v>R-WH_Det_GAS*</v>
       </c>
       <c r="E87" s="32" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F87" s="32" t="str">
         <f t="shared" si="9"/>
@@ -10557,7 +10557,7 @@
         <v>R-WH_Det_WOO*</v>
       </c>
       <c r="E90" s="33" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="F90" s="33" t="str">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
Debug - UC and start updating some boiler cost from AECOM
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\RSD22Feb21\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\RSD23Feb21\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4136AB88-F1C5-4A17-93BA-AC9BC249A269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA6DD8D-4EA1-4F3B-B199-CA885FF8B922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="-13740" windowWidth="21600" windowHeight="11385" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="-15810" windowWidth="21600" windowHeight="11385" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>

</xml_diff>

<commit_message>
Update - Sce and AFC Trans
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\RSD23Feb21\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA6DD8D-4EA1-4F3B-B199-CA885FF8B922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8465E3-C7C8-4B1F-9863-8AF107A2D3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="-15810" windowWidth="21600" windowHeight="11385" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>
@@ -5075,8 +5075,8 @@
   </sheetPr>
   <dimension ref="A1:L184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="B52" s="32" t="str">
         <f>"R-SW*"&amp;F52&amp;"_"&amp;G52&amp;",-*HPN*"</f>
@@ -6409,7 +6409,7 @@
       </c>
       <c r="D52" s="32">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H52,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.73685782056223E-2</v>
+        <v>3.19379469540736E-2</v>
       </c>
       <c r="F52" s="32" t="s">
         <v>109</v>
@@ -6418,8 +6418,8 @@
         <v>83</v>
       </c>
       <c r="H52" s="32" t="str">
-        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X1"</f>
-        <v>R-S*_Att_ELC*X1</v>
+        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X0"</f>
+        <v>R-S*_Att_ELC*X0</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -6760,7 +6760,7 @@
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="32" t="s">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="B66" s="32" t="str">
         <f>"R-SW*"&amp;F66&amp;"_"&amp;G66&amp;",-*HPN*"</f>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="D66" s="32">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H66,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.73685782056223E-2</v>
+        <v>3.19379469540736E-2</v>
       </c>
       <c r="F66" s="32" t="s">
         <v>105</v>
@@ -6781,8 +6781,8 @@
         <v>83</v>
       </c>
       <c r="H66" s="32" t="str">
-        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X1"</f>
-        <v>R-S*_Att_ELC*X1</v>
+        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X0"</f>
+        <v>R-S*_Att_ELC*X0</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7123,7 +7123,7 @@
     </row>
     <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="32" t="s">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="B80" s="32" t="str">
         <f>"R-SW*"&amp;F80&amp;"_"&amp;G80&amp;",-*HPN*"</f>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="D80" s="32">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H80,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.73685782056223E-2</v>
+        <v>3.19379469540736E-2</v>
       </c>
       <c r="F80" s="32" t="s">
         <v>114</v>
@@ -7144,8 +7144,8 @@
         <v>83</v>
       </c>
       <c r="H80" s="32" t="str">
-        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X1"</f>
-        <v>R-S*_Att_ELC*X1</v>
+        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X0"</f>
+        <v>R-S*_Att_ELC*X0</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update UC - Debug
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\RSD23Feb21\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2244A65C-7E6B-4C98-80F0-654A4EF26514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AC4FC2-E895-4AEC-A62A-C0410F2025D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="-14250" windowWidth="21600" windowHeight="11385" tabRatio="819" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>
@@ -1605,7 +1605,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1688,7 +1688,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2283,35 +2282,35 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37">
+      <c r="A4" s="36">
         <v>44237</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37">
+    <row r="5" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
         <v>44232</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="D5" s="36" t="str">
+      <c r="D5" s="35" t="str">
         <f>ADDRESS(ROW(AF!A3),COLUMN(AF!A3),4,1)&amp;","&amp;ADDRESS(ROW(AF!J3),COLUMN(AF!J3),4,1)&amp;","&amp;ADDRESS(ROW(AF!J15),COLUMN(AF!J15),4,1)</f>
         <v>A3,J3,J15</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="35" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5075,8 +5074,8 @@
   </sheetPr>
   <dimension ref="A1:L184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K93" sqref="K93"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5340,11 +5339,11 @@
       <c r="A11" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="B11" s="35" t="str">
+      <c r="B11" s="33" t="str">
         <f t="shared" ref="B11:B17" si="1">"R-SH*"&amp;F11&amp;"_"&amp;G11&amp;"*"</f>
         <v>R-SH*Apt_KER*</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="33">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H11,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>3.7359826231663999E-2</v>
@@ -6065,8 +6064,8 @@
         <v>262</v>
       </c>
       <c r="B38" s="32" t="str">
-        <f>"R-SH*"&amp;F38&amp;"_"&amp;G38&amp;"_N1"</f>
-        <v>R-SH*Det_ELC_N1</v>
+        <f>"R-SW*"&amp;F38&amp;"*"&amp;",-*HPN*"</f>
+        <v>R-SW*Det*,-*HPN*</v>
       </c>
       <c r="C38" s="32"/>
       <c r="D38" s="32">
@@ -6400,8 +6399,8 @@
         <v>206</v>
       </c>
       <c r="B52" s="32" t="str">
-        <f>"R-SW*"&amp;F52&amp;"_"&amp;G52&amp;",-*HPN*"</f>
-        <v>R-SW*Apt_ELC,-*HPN*</v>
+        <f>"R-SW*"&amp;F52&amp;"*"&amp;",-*HPN*"</f>
+        <v>R-SW*Apt*,-*HPN*</v>
       </c>
       <c r="C52" s="32" t="str">
         <f t="shared" si="8"/>
@@ -6409,7 +6408,7 @@
       </c>
       <c r="D52" s="32">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H52,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>3.19379469540736E-2</v>
+        <v>1.35582728420454E-2</v>
       </c>
       <c r="F52" s="32" t="s">
         <v>109</v>
@@ -6418,8 +6417,8 @@
         <v>83</v>
       </c>
       <c r="H52" s="32" t="str">
-        <f>"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"&amp;"X0"</f>
-        <v>R-S*_Att_ELC*X0</v>
+        <f>"R-S*_"&amp;F52&amp;"_"&amp;G52&amp;"_X0"</f>
+        <v>R-S*_Apt_ELC_X0</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -6763,8 +6762,8 @@
         <v>206</v>
       </c>
       <c r="B66" s="32" t="str">
-        <f>"R-SW*"&amp;F66&amp;"_"&amp;G66&amp;",-*HPN*"</f>
-        <v>R-SW*Att_ELC,-*HPN*</v>
+        <f>"R-SW*"&amp;F66&amp;"*"&amp;",-*HPN*"</f>
+        <v>R-SW*Att*,-*HPN*</v>
       </c>
       <c r="C66" s="32" t="str">
         <f t="shared" si="12"/>
@@ -6772,7 +6771,7 @@
       </c>
       <c r="D66" s="32">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H66,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
+        <v>3.19379469540736E-2</v>
       </c>
       <c r="F66" s="32" t="s">
         <v>105</v>
@@ -6781,8 +6780,8 @@
         <v>83</v>
       </c>
       <c r="H66" s="32" t="str">
-        <f>B66</f>
-        <v>R-SW*Att_ELC,-*HPN*</v>
+        <f>"R-S*_"&amp;F66&amp;"_"&amp;G66&amp;"_X0"</f>
+        <v>R-S*_Att_ELC_X0</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7126,8 +7125,8 @@
         <v>206</v>
       </c>
       <c r="B80" s="32" t="str">
-        <f>"R-SW*"&amp;F80&amp;"_"&amp;G80&amp;",-*HPN*"</f>
-        <v>R-SW*Det_ELC,-*HPN*</v>
+        <f>"R-SW*"&amp;F80&amp;"*"&amp;",-*HPN*"</f>
+        <v>R-SW*Det*,-*HPN*</v>
       </c>
       <c r="C80" s="32" t="str">
         <f t="shared" si="16"/>
@@ -7135,7 +7134,7 @@
       </c>
       <c r="D80" s="32">
         <f>SUMIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H80,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
+        <v>5.1441804976465701E-2</v>
       </c>
       <c r="F80" s="32" t="s">
         <v>114</v>
@@ -7144,8 +7143,8 @@
         <v>83</v>
       </c>
       <c r="H80" s="32" t="str">
-        <f>B80</f>
-        <v>R-SW*Det_ELC,-*HPN*</v>
+        <f>"R-S*_"&amp;F80&amp;"_"&amp;G80&amp;"_X0"</f>
+        <v>R-S*_Det_ELC_X0</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -8320,7 +8319,7 @@
         <v>R-WH_Det_SOL*</v>
       </c>
       <c r="C130" s="32"/>
-      <c r="D130" s="42">
+      <c r="D130" s="41">
         <f>SUMIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H130,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.113051511576835</v>
       </c>
@@ -9397,28 +9396,28 @@
       </c>
     </row>
     <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A172" s="38" t="s">
+      <c r="A172" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B172" s="38" t="str">
+      <c r="B172" s="37" t="str">
         <f t="shared" si="37"/>
         <v>R-SW_Det_SOL*</v>
       </c>
-      <c r="C172" s="38" t="str">
+      <c r="C172" s="37" t="str">
         <f t="shared" si="38"/>
         <v>RSDWH_Det</v>
       </c>
-      <c r="D172" s="38">
+      <c r="D172" s="37">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H172,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.113051511576835</v>
       </c>
-      <c r="F172" s="38" t="s">
+      <c r="F172" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="G172" s="38" t="s">
+      <c r="G172" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="H172" s="38" t="str">
+      <c r="H172" s="37" t="str">
         <f>"R-WH_"&amp;F172&amp;"_"&amp;G172&amp;"*"</f>
         <v>R-WH_Det_SOL*</v>
       </c>
@@ -9454,7 +9453,7 @@
       <c r="G174" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H174" s="39" t="str">
+      <c r="H174" s="38" t="str">
         <f t="shared" ref="H174:H176" si="41">"R-SH_"&amp;F174&amp;"_"&amp;G174&amp;"*X1"</f>
         <v>R-SH_Apt_ELC*X1</v>
       </c>
@@ -9478,7 +9477,7 @@
       <c r="G175" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H175" s="39" t="str">
+      <c r="H175" s="38" t="str">
         <f t="shared" si="41"/>
         <v>R-SH_Att_ELC*X1</v>
       </c>
@@ -9502,7 +9501,7 @@
       <c r="G176" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H176" s="39" t="str">
+      <c r="H176" s="38" t="str">
         <f t="shared" si="41"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
@@ -9541,7 +9540,7 @@
       <c r="G178" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H178" s="39" t="str">
+      <c r="H178" s="38" t="str">
         <f t="shared" ref="H178:H180" si="42">"R-SH_"&amp;F178&amp;"_"&amp;G178&amp;"*X1"</f>
         <v>R-SH_Apt_ELC*X1</v>
       </c>
@@ -9568,34 +9567,34 @@
       <c r="G179" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H179" s="39" t="str">
+      <c r="H179" s="38" t="str">
         <f t="shared" si="42"/>
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A180" s="40" t="s">
+      <c r="A180" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="B180" s="40" t="str">
+      <c r="B180" s="39" t="str">
         <f>"R-HC_"&amp;F180&amp;"_"&amp;G180&amp;"_HPN*"</f>
         <v>R-HC_Det_ELC_HPN*</v>
       </c>
-      <c r="C180" s="40" t="str">
+      <c r="C180" s="39" t="str">
         <f>"RSDSC_"&amp;F180</f>
         <v>RSDSC_Det</v>
       </c>
-      <c r="D180" s="40">
+      <c r="D180" s="39">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H180,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>3.17870115673878E-2</v>
       </c>
-      <c r="F180" s="40" t="s">
+      <c r="F180" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="G180" s="40" t="s">
+      <c r="G180" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="H180" s="41" t="str">
+      <c r="H180" s="40" t="str">
         <f t="shared" si="42"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
@@ -9667,28 +9666,28 @@
       </c>
     </row>
     <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A184" s="40" t="s">
+      <c r="A184" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="B184" s="40" t="str">
+      <c r="B184" s="39" t="str">
         <f>"R-HC_"&amp;F184&amp;"_"&amp;G184&amp;"_HPN*"</f>
         <v>R-HC_Det_ELC_HPN*</v>
       </c>
-      <c r="C184" s="40" t="str">
+      <c r="C184" s="39" t="str">
         <f>"RSDSH_"&amp;F184</f>
         <v>RSDSH_Det</v>
       </c>
-      <c r="D184" s="40">
+      <c r="D184" s="39">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H184,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>3.17870115673878E-2</v>
       </c>
-      <c r="F184" s="40" t="s">
+      <c r="F184" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="G184" s="40" t="s">
+      <c r="G184" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="H184" s="40" t="str">
+      <c r="H184" s="39" t="str">
         <f t="shared" si="43"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
@@ -9706,7 +9705,7 @@
   </sheetPr>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
@@ -10702,7 +10701,7 @@
       <c r="B48" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="39" t="str">
+      <c r="C48" s="38" t="str">
         <f>"R-SH_"&amp;A48&amp;"_"&amp;B48&amp;"*X1"</f>
         <v>R-SH_Apt_ELC*X1</v>
       </c>
@@ -10725,7 +10724,7 @@
       <c r="B49" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="39" t="str">
+      <c r="C49" s="38" t="str">
         <f>"R-SH_"&amp;A49&amp;"_"&amp;B49&amp;"*X1"</f>
         <v>R-SH_Att_ELC*X1</v>
       </c>
@@ -10742,24 +10741,24 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="40" t="s">
+      <c r="A50" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="41" t="str">
+      <c r="C50" s="40" t="str">
         <f>"R-SH_"&amp;A50&amp;"_"&amp;B50&amp;"*X1"</f>
         <v>R-SH_Det_ELC*X1</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="F50" s="40" t="str">
+      <c r="F50" s="39" t="str">
         <f t="shared" si="2"/>
         <v>R-SC_Det_ELC_N1</v>
       </c>
-      <c r="G50" s="40" t="str">
+      <c r="G50" s="39" t="str">
         <f>IFERROR("*"&amp;AVERAGEIFS('BY-RSD-EFF'!$L$2:$L$100,'BY-RSD-EFF'!$C$2:$C$100,EFF!C50,'BY-RSD-EFF'!$A$2:$A$100,"BASE"),"")</f>
         <v>*3.08978378378378</v>
       </c>
@@ -10896,7 +10895,7 @@
       <c r="B57" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="39" t="str">
+      <c r="C57" s="38" t="str">
         <f>"R-WH_"&amp;A57&amp;"_"&amp;B57&amp;"*X1"</f>
         <v>R-WH_Apt_ELC*X1</v>
       </c>
@@ -11205,7 +11204,7 @@
       <c r="B71" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="39" t="str">
+      <c r="C71" s="38" t="str">
         <f>"R-WH_"&amp;A71&amp;"_"&amp;B71&amp;"*X1"</f>
         <v>R-WH_Att_ELC*X1</v>
       </c>
@@ -11514,7 +11513,7 @@
       <c r="B85" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="39" t="str">
+      <c r="C85" s="38" t="str">
         <f>"R-WH_"&amp;A85&amp;"_"&amp;B85&amp;"*X1"</f>
         <v>R-WH_Det_ELC*X1</v>
       </c>
@@ -11702,7 +11701,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13362,6 +13361,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Introduce HOURLY VERSION - Introduce Hourly time slices - Introduce hourly Wind Onshore Availability factors - Introduce hourly Wind Offshore Availability factors - Introduce hourly Solar Availability factors - Introduce hourly Wave Availability factors - Introduce hourly Tidal Availability factors - Introduce hourly Hydro Availability factors
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VEDA_Models\2-NewVeda\TIMES-Ireland-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main-8760\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320BEF39-B02D-4599-B7F6-C02704756940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB88E2F-FF21-4829-B6A2-38F66A377395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{DF4C35E6-02C2-4233-84CE-A7CCAFFA4B20}"/>
+    <workbookView xWindow="5280" yWindow="3900" windowWidth="42165" windowHeight="23985" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7230" yWindow="5850" windowWidth="42165" windowHeight="23985" firstSheet="6" activeTab="6" xr2:uid="{DF4C35E6-02C2-4233-84CE-A7CCAFFA4B20}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>

</xml_diff>

<commit_message>
AFA Fireplace and HVO
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_Trans.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VEDA_Models\2-NewVeda\TIMES-Ireland-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320BEF39-B02D-4599-B7F6-C02704756940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B608DC-1C07-4F49-91A3-521CF5249FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{DF4C35E6-02C2-4233-84CE-A7CCAFFA4B20}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>
@@ -74,7 +73,7 @@
     <author>Alessandro Chiodi</author>
   </authors>
   <commentList>
-    <comment ref="D115" authorId="0" shapeId="0" xr:uid="{252C524F-867C-494B-8549-0779FBA2A96C}">
+    <comment ref="D123" authorId="0" shapeId="0" xr:uid="{252C524F-867C-494B-8549-0779FBA2A96C}">
       <text>
         <r>
           <rPr>
@@ -98,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H117" authorId="0" shapeId="0" xr:uid="{08155CC9-5232-4BA3-8E7D-2782073BC52D}">
+    <comment ref="H125" authorId="0" shapeId="0" xr:uid="{08155CC9-5232-4BA3-8E7D-2782073BC52D}">
       <text>
         <r>
           <rPr>
@@ -122,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H118" authorId="0" shapeId="0" xr:uid="{18A1B250-FDBD-4085-B842-EA94AB62C50C}">
+    <comment ref="H126" authorId="0" shapeId="0" xr:uid="{18A1B250-FDBD-4085-B842-EA94AB62C50C}">
       <text>
         <r>
           <rPr>
@@ -146,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H119" authorId="0" shapeId="0" xr:uid="{D04A0774-4BB1-4E99-9BCD-45E2F1A6AC6C}">
+    <comment ref="H127" authorId="0" shapeId="0" xr:uid="{D04A0774-4BB1-4E99-9BCD-45E2F1A6AC6C}">
       <text>
         <r>
           <rPr>
@@ -170,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H121" authorId="0" shapeId="0" xr:uid="{E2B5B631-C1AB-456E-AC2B-816F7B2C69C1}">
+    <comment ref="H129" authorId="0" shapeId="0" xr:uid="{E2B5B631-C1AB-456E-AC2B-816F7B2C69C1}">
       <text>
         <r>
           <rPr>
@@ -194,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H122" authorId="0" shapeId="0" xr:uid="{C376D617-8F0A-44E5-83D3-958CBFADFD31}">
+    <comment ref="H130" authorId="0" shapeId="0" xr:uid="{C376D617-8F0A-44E5-83D3-958CBFADFD31}">
       <text>
         <r>
           <rPr>
@@ -218,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H123" authorId="0" shapeId="0" xr:uid="{5B2CC33F-B70C-4EB5-AF3E-09C8B0B59273}">
+    <comment ref="H131" authorId="0" shapeId="0" xr:uid="{5B2CC33F-B70C-4EB5-AF3E-09C8B0B59273}">
       <text>
         <r>
           <rPr>
@@ -495,7 +494,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="277">
   <si>
     <t>IE</t>
   </si>
@@ -1320,6 +1319,30 @@
   </si>
   <si>
     <t>R-WH_Det_SOL_X0</t>
+  </si>
+  <si>
+    <t>R-SH_Att_FPL*</t>
+  </si>
+  <si>
+    <t>R-SH_Det_FPL*</t>
+  </si>
+  <si>
+    <t>R-SW_Att_FPL*</t>
+  </si>
+  <si>
+    <t>R-SW_Det_FPL*</t>
+  </si>
+  <si>
+    <t>R-SH_Att_HVO*</t>
+  </si>
+  <si>
+    <t>R-SH_Det_HVO*</t>
+  </si>
+  <si>
+    <t>R-SW_Att_HVO*</t>
+  </si>
+  <si>
+    <t>R-SW_Det_HVO*</t>
   </si>
 </sst>
 </file>
@@ -2239,7 +2262,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2311,9 +2333,6 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="M43" sqref="M43"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2409,7 +2428,6 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2587,7 +2605,6 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2685,7 +2702,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2866,7 +2882,6 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2962,9 +2977,6 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3144,7 +3156,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3242,7 +3253,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3341,7 +3351,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4109,7 +4118,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4306,7 +4314,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5155,12 +5162,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5789,7 +5795,7 @@
         <v>244</v>
       </c>
       <c r="B23" s="33" t="str">
-        <f t="shared" ref="B23:B28" si="3">"R-SH*"&amp;F23&amp;"_"&amp;G23&amp;"*"</f>
+        <f t="shared" ref="B23:B30" si="3">"R-SH*"&amp;F23&amp;"_"&amp;G23&amp;"*"</f>
         <v>R-SH*Att_KER*</v>
       </c>
       <c r="C23" s="33"/>
@@ -5819,185 +5825,171 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="B24" s="32" t="str">
+      <c r="B24" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33">
+        <f>D23</f>
+        <v>3.5982700943281098E-2</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="32" t="str">
         <f t="shared" si="3"/>
         <v>R-SH*Att_GAS*</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H24,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H25,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>2.8026244703222701E-2</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F25" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G25" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="H24" s="32" t="str">
-        <f>"R-S*_"&amp;F23&amp;"_"&amp;G24&amp;"*"</f>
+      <c r="H25" s="32" t="str">
+        <f>"R-S*_"&amp;F23&amp;"_"&amp;G25&amp;"*"</f>
         <v>R-S*_Att_GAS*</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="33" t="str">
+      <c r="B26" s="33" t="str">
         <f t="shared" si="3"/>
         <v>R-SH*Att_PEA*</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H25,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H26,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>5.6714843841128501E-2</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F26" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G26" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="H25" s="33" t="str">
-        <f>"R-S*_"&amp;F25&amp;"_"&amp;G25&amp;"*"</f>
+      <c r="H26" s="33" t="str">
+        <f>"R-S*_"&amp;F26&amp;"_"&amp;G26&amp;"*"</f>
         <v>R-S*_Att_PEA*</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="32" t="str">
+      <c r="B27" s="32" t="str">
         <f t="shared" si="3"/>
         <v>R-SH*Att_SMF*</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H26,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H27,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>5.8905144753244799E-2</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F27" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G27" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="H26" s="32" t="str">
-        <f>"R-S*_"&amp;F26&amp;"_"&amp;G26&amp;"*"</f>
+      <c r="H27" s="32" t="str">
+        <f>"R-S*_"&amp;F27&amp;"_"&amp;G27&amp;"*"</f>
         <v>R-S*_Att_SMF*</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="B27" s="33" t="str">
-        <f t="shared" si="3"/>
+      <c r="B28" s="33" t="str">
+        <f>"R-SH*"&amp;F28&amp;"_"&amp;G28&amp;"*"</f>
         <v>R-SH*Att_WOO*</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H27,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H28,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>9.52141887785493E-2</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F28" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G28" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H27" s="33" t="str">
-        <f>"R-S*_"&amp;F27&amp;"_"&amp;G27&amp;"*"</f>
+      <c r="H28" s="33" t="str">
+        <f>"R-S*_"&amp;F28&amp;"_"&amp;G28&amp;"*"</f>
         <v>R-S*_Att_WOO*</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="32" t="str">
-        <f t="shared" si="3"/>
-        <v>R-SH*Att_HET*</v>
-      </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H28,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.82983145664136E-2</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" s="32" t="str">
-        <f>"R-S*_"&amp;F28&amp;"_"&amp;G28&amp;"*"</f>
-        <v>R-S*_Att_HET*</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33">
+        <f>D28</f>
+        <v>9.52141887785493E-2</v>
+      </c>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
     </row>
     <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="32" t="str">
-        <f>"R-SH*"&amp;F30&amp;"_"&amp;G30&amp;"*"</f>
-        <v>R-SH*Det_COA*</v>
+        <f t="shared" si="3"/>
+        <v>R-SH*Att_HET*</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H30,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.56734094210587305</v>
+        <v>1.82983145664136E-2</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H30" s="32" t="str">
-        <f t="shared" ref="H30:H33" si="5">"R-S*_"&amp;F30&amp;"_"&amp;G30&amp;"*"</f>
-        <v>R-S*_Det_COA*</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="33" t="str">
-        <f>"R-SH*"&amp;F31&amp;"_"&amp;G31&amp;"*"</f>
-        <v>R-SH*Det_BDL*</v>
-      </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H31,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H31" s="33" t="str">
-        <f t="shared" si="5"/>
-        <v>R-S*_Det_BDL*</v>
-      </c>
-      <c r="I31" s="25"/>
+        <f>"R-S*_"&amp;F30&amp;"_"&amp;G30&amp;"*"</f>
+        <v>R-S*_Att_HET*</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
     </row>
     <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
@@ -6005,468 +5997,441 @@
       </c>
       <c r="B32" s="32" t="str">
         <f>"R-SH*"&amp;F32&amp;"_"&amp;G32&amp;"*"</f>
-        <v>R-SH*Det_ETH*</v>
+        <v>R-SH*Det_COA*</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H32,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
+        <v>0.56734094210587305</v>
       </c>
       <c r="F32" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="H32" s="32" t="str">
-        <f t="shared" si="5"/>
-        <v>R-S*_Det_ETH*</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H32:H35" si="5">"R-S*_"&amp;F32&amp;"_"&amp;G32&amp;"*"</f>
+        <v>R-S*_Det_COA*</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="B33" s="33" t="str">
         <f>"R-SH*"&amp;F33&amp;"_"&amp;G33&amp;"*"</f>
-        <v>R-SH*Det_LPG*</v>
+        <v>R-SH*Det_BDL*</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="33">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H33,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>8.5024956709859906E-2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="33" t="s">
         <v>114</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" si="5"/>
-        <v>R-S*_Det_LPG*</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>R-S*_Det_BDL*</v>
+      </c>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="B34" s="32" t="str">
         <f>"R-SH*"&amp;F34&amp;"_"&amp;G34&amp;"*"</f>
-        <v>R-SH*Det_ELC*</v>
+        <v>R-SH*Det_ETH*</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H34,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>5.2637209370950108E-2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="H34" s="32" t="str">
-        <f>"R-S*_"&amp;F34&amp;"_"&amp;G34&amp;"*"</f>
-        <v>R-S*_Det_ELC*</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>R-S*_Det_ETH*</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>244</v>
       </c>
       <c r="B35" s="33" t="str">
-        <f t="shared" ref="B35:B40" si="6">"R-SH*"&amp;F35&amp;"_"&amp;G35&amp;"*"</f>
-        <v>R-SH*Det_KER*</v>
+        <f>"R-SH*"&amp;F35&amp;"_"&amp;G35&amp;"*"</f>
+        <v>R-SH*Det_LPG*</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="33">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H35,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>5.9134611842239497E-2</v>
+        <v>8.5024956709859906E-2</v>
       </c>
       <c r="F35" s="33" t="s">
         <v>114</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H35" s="33" t="str">
-        <f t="shared" ref="H35" si="7">"R-S*_"&amp;F35&amp;"_"&amp;G35&amp;"*"</f>
-        <v>R-S*_Det_KER*</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>R-S*_Det_LPG*</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>244</v>
       </c>
       <c r="B36" s="32" t="str">
-        <f t="shared" si="6"/>
-        <v>R-SH*Det_GAS*</v>
+        <f>"R-SH*"&amp;F36&amp;"_"&amp;G36&amp;"*"</f>
+        <v>R-SH*Det_ELC*</v>
       </c>
       <c r="C36" s="32"/>
       <c r="D36" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H36,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>4.6982028361355302E-2</v>
+        <v>5.2637209370950108E-2</v>
       </c>
       <c r="F36" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>194</v>
+        <v>83</v>
       </c>
       <c r="H36" s="32" t="str">
-        <f>"R-S*_"&amp;F35&amp;"_"&amp;G36&amp;"*"</f>
-        <v>R-S*_Det_GAS*</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <f>"R-S*_"&amp;F36&amp;"_"&amp;G36&amp;"*"</f>
+        <v>R-S*_Det_ELC*</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="B37" s="33" t="str">
-        <f t="shared" si="6"/>
-        <v>R-SH*Det_PEA*</v>
+        <f t="shared" ref="B37:B44" si="6">"R-SH*"&amp;F37&amp;"_"&amp;G37&amp;"*"</f>
+        <v>R-SH*Det_KER*</v>
       </c>
       <c r="C37" s="33"/>
       <c r="D37" s="33">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H37,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.120504252519882</v>
+        <v>5.9134611842239497E-2</v>
       </c>
       <c r="F37" s="33" t="s">
         <v>114</v>
       </c>
       <c r="G37" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H37" s="33" t="str">
+        <f t="shared" ref="H37" si="7">"R-S*_"&amp;F37&amp;"_"&amp;G37&amp;"*"</f>
+        <v>R-S*_Det_KER*</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33">
+        <f>D37</f>
+        <v>5.9134611842239497E-2</v>
+      </c>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B39" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>R-SH*Det_GAS*</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H39,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>4.6982028361355302E-2</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="H39" s="32" t="str">
+        <f>"R-S*_"&amp;F37&amp;"_"&amp;G39&amp;"*"</f>
+        <v>R-S*_Det_GAS*</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>R-SH*Det_PEA*</v>
+      </c>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H40,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>0.120504252519882</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="33" t="str">
-        <f>"R-S*_"&amp;F37&amp;"_"&amp;G37&amp;"*"</f>
+      <c r="H40" s="33" t="str">
+        <f>"R-S*_"&amp;F40&amp;"_"&amp;G40&amp;"*"</f>
         <v>R-S*_Det_PEA*</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="32" t="str">
+      <c r="B41" s="32" t="str">
         <f t="shared" si="6"/>
         <v>R-SH*Det_SMF*</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H38,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H41,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.16465051297265201</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F41" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="G38" s="32" t="s">
+      <c r="G41" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="H38" s="32" t="str">
-        <f>"R-S*_"&amp;F38&amp;"_"&amp;G38&amp;"*"</f>
+      <c r="H41" s="32" t="str">
+        <f>"R-S*_"&amp;F41&amp;"_"&amp;G41&amp;"*"</f>
         <v>R-S*_Det_SMF*</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="B39" s="33" t="str">
+      <c r="B42" s="33" t="str">
         <f t="shared" si="6"/>
         <v>R-SH*Det_WOO*</v>
       </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H39,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H42,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.115618760253806</v>
       </c>
-      <c r="F39" s="33" t="s">
+      <c r="F42" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G42" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H39" s="33" t="str">
-        <f>"R-S*_"&amp;F39&amp;"_"&amp;G39&amp;"*"</f>
+      <c r="H42" s="33" t="str">
+        <f>"R-S*_"&amp;F42&amp;"_"&amp;G42&amp;"*"</f>
         <v>R-S*_Det_WOO*</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33">
+        <f>D42</f>
+        <v>0.115618760253806</v>
+      </c>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+    </row>
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="32" t="str">
+      <c r="B44" s="32" t="str">
         <f t="shared" si="6"/>
         <v>R-SH*Det_HET*</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H40,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H44,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>0.24099011008044599</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F44" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="G40" s="32" t="s">
+      <c r="G44" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="32" t="str">
-        <f>"R-S*_"&amp;F40&amp;"_"&amp;G40&amp;"*"</f>
+      <c r="H44" s="32" t="str">
+        <f>"R-S*_"&amp;F44&amp;"_"&amp;G44&amp;"*"</f>
         <v>R-S*_Det_HET*</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
         <v>1</v>
-      </c>
-      <c r="B42" s="32" t="str">
-        <f>"R-SW*"&amp;F42&amp;"_"&amp;G42&amp;"*"</f>
-        <v>R-SW*Apt_COA*</v>
-      </c>
-      <c r="C42" s="32" t="str">
-        <f t="shared" ref="C42:C52" si="8">"RSDSH_"&amp;F42&amp;",RSDWH_"&amp;F54</f>
-        <v>RSDSH_Apt,RSDWH_Att</v>
-      </c>
-      <c r="D42" s="32">
-        <f t="shared" ref="D42:D52" si="9">AVERAGE(D6,D78)</f>
-        <v>0.1528008913749376</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G42" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="H42" s="32" t="str">
-        <f t="shared" ref="H42:H45" si="10">"R-S*_"&amp;F42&amp;"_"&amp;G42&amp;"*"</f>
-        <v>R-S*_Apt_COA*</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="33" t="str">
-        <f>"R-SW*"&amp;F43&amp;"_"&amp;G43&amp;"*"</f>
-        <v>R-SW*Apt_BDL*</v>
-      </c>
-      <c r="C43" s="33" t="str">
-        <f t="shared" si="8"/>
-        <v>RSDSH_Apt,RSDWH_Att</v>
-      </c>
-      <c r="D43" s="33">
-        <f t="shared" si="9"/>
-        <v>7.3402048028933953E-3</v>
-      </c>
-      <c r="F43" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G43" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H43" s="33" t="str">
-        <f t="shared" si="10"/>
-        <v>R-S*_Apt_BDL*</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="32" t="str">
-        <f>"R-SW*"&amp;F44&amp;"_"&amp;G44&amp;"*"</f>
-        <v>R-SW*Apt_ETH*</v>
-      </c>
-      <c r="C44" s="32" t="str">
-        <f t="shared" si="8"/>
-        <v>RSDSH_Apt,RSDWH_Att</v>
-      </c>
-      <c r="D44" s="32">
-        <f t="shared" si="9"/>
-        <v>5.4314481815592374E-3</v>
-      </c>
-      <c r="F44" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G44" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H44" s="32" t="str">
-        <f t="shared" si="10"/>
-        <v>R-S*_Apt_ETH*</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B45" s="33" t="str">
-        <f>"R-SW*"&amp;F45&amp;"_"&amp;G45&amp;"*"</f>
-        <v>R-SW*Apt_LPG*</v>
-      </c>
-      <c r="C45" s="33" t="str">
-        <f t="shared" si="8"/>
-        <v>RSDSH_Apt,RSDWH_Att</v>
-      </c>
-      <c r="D45" s="33">
-        <f t="shared" si="9"/>
-        <v>2.2587406471325601E-2</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G45" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="H45" s="33" t="str">
-        <f t="shared" si="10"/>
-        <v>R-S*_Apt_LPG*</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
-        <v>198</v>
       </c>
       <c r="B46" s="32" t="str">
         <f>"R-SW*"&amp;F46&amp;"_"&amp;G46&amp;"*"</f>
-        <v>R-SW*Apt_ELC*</v>
+        <v>R-SW*Apt_COA*</v>
       </c>
       <c r="C46" s="32" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F46&amp;",RSDWH_"&amp;F58</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D46" s="32">
-        <f t="shared" si="9"/>
-        <v>2.5406290924250299E-2</v>
+        <f>AVERAGE(D6,D86)</f>
+        <v>0.1528008913749376</v>
       </c>
       <c r="F46" s="32" t="s">
         <v>109</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H46" s="32" t="str">
-        <f>"R-S*_"&amp;F46&amp;"_"&amp;G46&amp;"*"</f>
-        <v>R-S*_Apt_ELC*</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H46:H49" si="8">"R-S*_"&amp;F46&amp;"_"&amp;G46&amp;"*"</f>
+        <v>R-S*_Apt_COA*</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B47" s="33" t="str">
-        <f t="shared" ref="B47:B52" si="11">"R-SW*"&amp;F47&amp;"_"&amp;G47&amp;"*"</f>
-        <v>R-SW*Apt_KER*</v>
+        <f>"R-SW*"&amp;F47&amp;"_"&amp;G47&amp;"*"</f>
+        <v>R-SW*Apt_BDL*</v>
       </c>
       <c r="C47" s="33" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F47&amp;",RSDWH_"&amp;F59</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D47" s="33">
-        <f t="shared" si="9"/>
-        <v>3.0423648377750551E-2</v>
+        <f>AVERAGE(D7,D87)</f>
+        <v>7.3402048028933953E-3</v>
       </c>
       <c r="F47" s="33" t="s">
         <v>109</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H47" s="33" t="str">
-        <f t="shared" ref="H47" si="12">"R-S*_"&amp;F47&amp;"_"&amp;G47&amp;"*"</f>
-        <v>R-S*_Apt_KER*</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>R-S*_Apt_BDL*</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B48" s="32" t="str">
-        <f t="shared" si="11"/>
-        <v>R-SW*Apt_GAS*</v>
+        <f>"R-SW*"&amp;F48&amp;"_"&amp;G48&amp;"*"</f>
+        <v>R-SW*Apt_ETH*</v>
       </c>
       <c r="C48" s="32" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F48&amp;",RSDWH_"&amp;F60</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D48" s="32">
-        <f t="shared" si="9"/>
-        <v>1.2023720455024919E-2</v>
+        <f>AVERAGE(D8,D88)</f>
+        <v>5.4314481815592374E-3</v>
       </c>
       <c r="F48" s="32" t="s">
         <v>109</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H48" s="32" t="str">
-        <f>"R-S*_"&amp;F47&amp;"_"&amp;G48&amp;"*"</f>
-        <v>R-S*_Apt_GAS*</v>
+        <f t="shared" si="8"/>
+        <v>R-S*_Apt_ETH*</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B49" s="33" t="str">
-        <f t="shared" si="11"/>
-        <v>R-SW*Apt_PEA*</v>
+        <f>"R-SW*"&amp;F49&amp;"_"&amp;G49&amp;"*"</f>
+        <v>R-SW*Apt_LPG*</v>
       </c>
       <c r="C49" s="33" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F49&amp;",RSDWH_"&amp;F61</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D49" s="33">
-        <f t="shared" si="9"/>
-        <v>5.2921783539597103E-2</v>
+        <f>AVERAGE(D9,D89)</f>
+        <v>2.2587406471325601E-2</v>
       </c>
       <c r="F49" s="33" t="s">
         <v>109</v>
       </c>
       <c r="G49" s="33" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="H49" s="33" t="str">
-        <f>"R-S*_"&amp;F49&amp;"_"&amp;G49&amp;"*"</f>
-        <v>R-S*_Apt_PEA*</v>
+        <f t="shared" si="8"/>
+        <v>R-S*_Apt_LPG*</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B50" s="32" t="str">
-        <f t="shared" si="11"/>
-        <v>R-SW*Apt_SMF*</v>
+        <f>"R-SW*"&amp;F50&amp;"_"&amp;G50&amp;"*"</f>
+        <v>R-SW*Apt_ELC*</v>
       </c>
       <c r="C50" s="32" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F50&amp;",RSDWH_"&amp;F62</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D50" s="32">
-        <f t="shared" si="9"/>
-        <v>4.9506675305099501E-2</v>
+        <f>AVERAGE(D10,D90)</f>
+        <v>2.5406290924250299E-2</v>
       </c>
       <c r="F50" s="32" t="s">
         <v>109</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="H50" s="32" t="str">
         <f>"R-S*_"&amp;F50&amp;"_"&amp;G50&amp;"*"</f>
-        <v>R-S*_Apt_SMF*</v>
+        <v>R-S*_Apt_ELC*</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -6474,26 +6439,26 @@
         <v>198</v>
       </c>
       <c r="B51" s="33" t="str">
-        <f t="shared" si="11"/>
-        <v>R-SW*Apt_WOO*</v>
+        <f t="shared" ref="B51:B56" si="9">"R-SW*"&amp;F51&amp;"_"&amp;G51&amp;"*"</f>
+        <v>R-SW*Apt_KER*</v>
       </c>
       <c r="C51" s="33" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F51&amp;",RSDWH_"&amp;F63</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D51" s="33">
-        <f t="shared" si="9"/>
-        <v>1.738190021295305E-2</v>
+        <f>AVERAGE(D11,D91)</f>
+        <v>3.0423648377750551E-2</v>
       </c>
       <c r="F51" s="33" t="s">
         <v>109</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H51" s="33" t="str">
-        <f>"R-S*_"&amp;F51&amp;"_"&amp;G51&amp;"*"</f>
-        <v>R-S*_Apt_WOO*</v>
+        <f t="shared" ref="H51" si="10">"R-S*_"&amp;F51&amp;"_"&amp;G51&amp;"*"</f>
+        <v>R-S*_Apt_KER*</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -6501,281 +6466,281 @@
         <v>198</v>
       </c>
       <c r="B52" s="32" t="str">
-        <f t="shared" si="11"/>
-        <v>R-SW*Apt_HET*</v>
+        <f t="shared" si="9"/>
+        <v>R-SW*Apt_GAS*</v>
       </c>
       <c r="C52" s="32" t="str">
-        <f t="shared" si="8"/>
+        <f>"RSDSH_"&amp;F52&amp;",RSDWH_"&amp;F65</f>
         <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D52" s="32">
-        <f t="shared" si="9"/>
-        <v>8.9890643927955554E-4</v>
+        <f>AVERAGE(D12,D92)</f>
+        <v>1.2023720455024919E-2</v>
       </c>
       <c r="F52" s="32" t="s">
         <v>109</v>
       </c>
       <c r="G52" s="32" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
       <c r="H52" s="32" t="str">
-        <f>"R-S*_"&amp;F52&amp;"_"&amp;G52&amp;"*"</f>
-        <v>R-S*_Apt_HET*</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
+        <f>"R-S*_"&amp;F51&amp;"_"&amp;G52&amp;"*"</f>
+        <v>R-S*_Apt_GAS*</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="33" t="str">
+        <f t="shared" si="9"/>
+        <v>R-SW*Apt_PEA*</v>
+      </c>
+      <c r="C53" s="33" t="str">
+        <f>"RSDSH_"&amp;F53&amp;",RSDWH_"&amp;F66</f>
+        <v>RSDSH_Apt,RSDWH_Att</v>
+      </c>
+      <c r="D53" s="33">
+        <f>AVERAGE(D13,D93)</f>
+        <v>5.2921783539597103E-2</v>
+      </c>
+      <c r="F53" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H53" s="33" t="str">
+        <f>"R-S*_"&amp;F53&amp;"_"&amp;G53&amp;"*"</f>
+        <v>R-S*_Apt_PEA*</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="32" t="str">
-        <f>"R-SW*"&amp;F54&amp;"_"&amp;G54&amp;"*"</f>
-        <v>R-SW*Att_COA*</v>
+        <f t="shared" si="9"/>
+        <v>R-SW*Apt_SMF*</v>
       </c>
       <c r="C54" s="32" t="str">
-        <f>"RSDSH_"&amp;F54&amp;",RSDWH_"&amp;F54</f>
-        <v>RSDSH_Att,RSDWH_Att</v>
+        <f>"RSDSH_"&amp;F54&amp;",RSDWH_"&amp;F67</f>
+        <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D54" s="32">
-        <f t="shared" ref="D54:D64" si="13">AVERAGE(D18,D91)</f>
-        <v>0.13757508933389442</v>
+        <f>AVERAGE(D14,D94)</f>
+        <v>4.9506675305099501E-2</v>
       </c>
       <c r="F54" s="32" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G54" s="32" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="H54" s="32" t="str">
-        <f t="shared" ref="H54:H57" si="14">"R-S*_"&amp;F54&amp;"_"&amp;G54&amp;"*"</f>
-        <v>R-S*_Att_COA*</v>
+        <f>"R-S*_"&amp;F54&amp;"_"&amp;G54&amp;"*"</f>
+        <v>R-S*_Apt_SMF*</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B55" s="33" t="str">
-        <f>"R-SW*"&amp;F55&amp;"_"&amp;G55&amp;"*"</f>
-        <v>R-SW*Att_BDL*</v>
+        <f t="shared" si="9"/>
+        <v>R-SW*Apt_WOO*</v>
       </c>
       <c r="C55" s="33" t="str">
-        <f t="shared" ref="C55:C64" si="15">"RSDSH_"&amp;F55&amp;",RSDWH_"&amp;F55</f>
-        <v>RSDSH_Att,RSDWH_Att</v>
+        <f>"RSDSH_"&amp;F55&amp;",RSDWH_"&amp;F68</f>
+        <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D55" s="33">
-        <f t="shared" si="13"/>
-        <v>1.8755504737112953E-2</v>
+        <f>AVERAGE(D15,D95)</f>
+        <v>1.738190021295305E-2</v>
       </c>
       <c r="F55" s="33" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G55" s="33" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H55" s="33" t="str">
-        <f t="shared" si="14"/>
-        <v>R-S*_Att_BDL*</v>
+        <f>"R-S*_"&amp;F55&amp;"_"&amp;G55&amp;"*"</f>
+        <v>R-S*_Apt_WOO*</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B56" s="32" t="str">
-        <f>"R-SW*"&amp;F56&amp;"_"&amp;G56&amp;"*"</f>
-        <v>R-SW*Att_ETH*</v>
+        <f t="shared" si="9"/>
+        <v>R-SW*Apt_HET*</v>
       </c>
       <c r="C56" s="32" t="str">
-        <f t="shared" si="15"/>
-        <v>RSDSH_Att,RSDWH_Att</v>
+        <f t="shared" ref="C56" si="11">"RSDSH_"&amp;F56&amp;",RSDWH_"&amp;F70</f>
+        <v>RSDSH_Apt,RSDWH_Att</v>
       </c>
       <c r="D56" s="32">
-        <f t="shared" si="13"/>
-        <v>6.72123287671235E-3</v>
+        <f>AVERAGE(D16,D96)</f>
+        <v>8.9890643927955554E-4</v>
       </c>
       <c r="F56" s="32" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G56" s="32" t="s">
-        <v>190</v>
+        <v>84</v>
       </c>
       <c r="H56" s="32" t="str">
-        <f t="shared" si="14"/>
-        <v>R-S*_Att_ETH*</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B57" s="33" t="str">
-        <f>"R-SW*"&amp;F57&amp;"_"&amp;G57&amp;"*"</f>
-        <v>R-SW*Att_LPG*</v>
-      </c>
-      <c r="C57" s="33" t="str">
-        <f t="shared" si="15"/>
-        <v>RSDSH_Att,RSDWH_Att</v>
-      </c>
-      <c r="D57" s="33">
-        <f t="shared" si="13"/>
-        <v>2.9676777946404852E-2</v>
-      </c>
-      <c r="F57" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="H57" s="33" t="str">
-        <f t="shared" si="14"/>
-        <v>R-S*_Att_LPG*</v>
-      </c>
+        <f>"R-S*_"&amp;F56&amp;"_"&amp;G56&amp;"*"</f>
+        <v>R-S*_Apt_HET*</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A57" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30"/>
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B58" s="32" t="str">
         <f>"R-SW*"&amp;F58&amp;"_"&amp;G58&amp;"*"</f>
-        <v>R-SW*Att_ELC*</v>
+        <v>R-SW*Att_COA*</v>
       </c>
       <c r="C58" s="32" t="str">
-        <f t="shared" si="15"/>
+        <f>"RSDSH_"&amp;F58&amp;",RSDWH_"&amp;F58</f>
         <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D58" s="32">
-        <f t="shared" si="13"/>
-        <v>2.3774911335309026E-2</v>
+        <f>AVERAGE(D18,D99)</f>
+        <v>0.13757508933389442</v>
       </c>
       <c r="F58" s="32" t="s">
         <v>105</v>
       </c>
       <c r="G58" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H58" s="32" t="str">
-        <f>"R-S*_"&amp;F58&amp;"_"&amp;G58&amp;"*"</f>
-        <v>R-S*_Att_ELC*</v>
+        <f t="shared" ref="H58:H61" si="12">"R-S*_"&amp;F58&amp;"_"&amp;G58&amp;"*"</f>
+        <v>R-S*_Att_COA*</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B59" s="33" t="str">
-        <f t="shared" ref="B59:B64" si="16">"R-SW*"&amp;F59&amp;"_"&amp;G59&amp;"*"</f>
-        <v>R-SW*Att_KER*</v>
+        <f>"R-SW*"&amp;F59&amp;"_"&amp;G59&amp;"*"</f>
+        <v>R-SW*Att_BDL*</v>
       </c>
       <c r="C59" s="33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="C59:C70" si="13">"RSDSH_"&amp;F59&amp;",RSDWH_"&amp;F59</f>
         <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D59" s="33">
-        <f t="shared" si="13"/>
-        <v>2.4961878258338448E-2</v>
+        <f>AVERAGE(D19,D100)</f>
+        <v>1.8755504737112953E-2</v>
       </c>
       <c r="F59" s="33" t="s">
         <v>105</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H59" s="33" t="str">
-        <f t="shared" ref="H59" si="17">"R-S*_"&amp;F59&amp;"_"&amp;G59&amp;"*"</f>
-        <v>R-S*_Att_KER*</v>
+        <f t="shared" si="12"/>
+        <v>R-S*_Att_BDL*</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B60" s="32" t="str">
-        <f t="shared" si="16"/>
-        <v>R-SW*Att_GAS*</v>
+        <f>"R-SW*"&amp;F60&amp;"_"&amp;G60&amp;"*"</f>
+        <v>R-SW*Att_ETH*</v>
       </c>
       <c r="C60" s="32" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D60" s="32">
-        <f t="shared" si="13"/>
-        <v>1.9851979150358402E-2</v>
+        <f>AVERAGE(D20,D101)</f>
+        <v>6.72123287671235E-3</v>
       </c>
       <c r="F60" s="32" t="s">
         <v>105</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H60" s="32" t="str">
-        <f>"R-S*_"&amp;F59&amp;"_"&amp;G60&amp;"*"</f>
-        <v>R-S*_Att_GAS*</v>
+        <f t="shared" si="12"/>
+        <v>R-S*_Att_ETH*</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B61" s="33" t="str">
-        <f t="shared" si="16"/>
-        <v>R-SW*Att_PEA*</v>
+        <f>"R-SW*"&amp;F61&amp;"_"&amp;G61&amp;"*"</f>
+        <v>R-SW*Att_LPG*</v>
       </c>
       <c r="C61" s="33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D61" s="33">
-        <f t="shared" si="13"/>
-        <v>3.5251852813074448E-2</v>
+        <f>AVERAGE(D21,D102)</f>
+        <v>2.9676777946404852E-2</v>
       </c>
       <c r="F61" s="33" t="s">
         <v>105</v>
       </c>
       <c r="G61" s="33" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="H61" s="33" t="str">
-        <f>"R-S*_"&amp;F61&amp;"_"&amp;G61&amp;"*"</f>
-        <v>R-S*_Att_PEA*</v>
+        <f t="shared" si="12"/>
+        <v>R-S*_Att_LPG*</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B62" s="32" t="str">
-        <f t="shared" si="16"/>
-        <v>R-SW*Att_SMF*</v>
+        <f>"R-SW*"&amp;F62&amp;"_"&amp;G62&amp;"*"</f>
+        <v>R-SW*Att_ELC*</v>
       </c>
       <c r="C62" s="32" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D62" s="32">
-        <f t="shared" si="13"/>
-        <v>3.5356636251858302E-2</v>
+        <f>AVERAGE(D22,D103)</f>
+        <v>2.3774911335309026E-2</v>
       </c>
       <c r="F62" s="32" t="s">
         <v>105</v>
       </c>
       <c r="G62" s="32" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="H62" s="32" t="str">
         <f>"R-S*_"&amp;F62&amp;"_"&amp;G62&amp;"*"</f>
-        <v>R-S*_Att_SMF*</v>
+        <v>R-S*_Att_ELC*</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -6783,254 +6748,238 @@
         <v>198</v>
       </c>
       <c r="B63" s="33" t="str">
-        <f t="shared" si="16"/>
-        <v>R-SW*Att_WOO*</v>
+        <f t="shared" ref="B63:B70" si="14">"R-SW*"&amp;F63&amp;"_"&amp;G63&amp;"*"</f>
+        <v>R-SW*Att_KER*</v>
       </c>
       <c r="C63" s="33" t="str">
-        <f t="shared" si="15"/>
+        <f>"RSDSH_"&amp;F63&amp;",RSDWH_"&amp;F63</f>
         <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D63" s="33">
-        <f t="shared" si="13"/>
-        <v>5.4484908352032999E-2</v>
+        <f>AVERAGE(D23,D104)</f>
+        <v>2.4961878258338448E-2</v>
       </c>
       <c r="F63" s="33" t="s">
         <v>105</v>
       </c>
       <c r="G63" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H63" s="33" t="str">
+        <f t="shared" ref="H63" si="15">"R-S*_"&amp;F63&amp;"_"&amp;G63&amp;"*"</f>
+        <v>R-S*_Att_KER*</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="C64" s="33" t="str">
+        <f>"RSDSH_"&amp;F63&amp;",RSDWH_"&amp;F63</f>
+        <v>RSDSH_Att,RSDWH_Att</v>
+      </c>
+      <c r="D64" s="33">
+        <f>D63</f>
+        <v>2.4961878258338448E-2</v>
+      </c>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+    </row>
+    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B65" s="32" t="str">
+        <f t="shared" si="14"/>
+        <v>R-SW*Att_GAS*</v>
+      </c>
+      <c r="C65" s="32" t="str">
+        <f t="shared" si="13"/>
+        <v>RSDSH_Att,RSDWH_Att</v>
+      </c>
+      <c r="D65" s="32">
+        <f>AVERAGE(D25,D105)</f>
+        <v>1.9851979150358402E-2</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="H65" s="32" t="str">
+        <f>"R-S*_"&amp;F63&amp;"_"&amp;G65&amp;"*"</f>
+        <v>R-S*_Att_GAS*</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="33" t="str">
+        <f t="shared" si="14"/>
+        <v>R-SW*Att_PEA*</v>
+      </c>
+      <c r="C66" s="33" t="str">
+        <f t="shared" si="13"/>
+        <v>RSDSH_Att,RSDWH_Att</v>
+      </c>
+      <c r="D66" s="33">
+        <f>AVERAGE(D26,D106)</f>
+        <v>3.5251852813074448E-2</v>
+      </c>
+      <c r="F66" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G66" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H66" s="33" t="str">
+        <f>"R-S*_"&amp;F66&amp;"_"&amp;G66&amp;"*"</f>
+        <v>R-S*_Att_PEA*</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="32" t="str">
+        <f t="shared" si="14"/>
+        <v>R-SW*Att_SMF*</v>
+      </c>
+      <c r="C67" s="32" t="str">
+        <f t="shared" si="13"/>
+        <v>RSDSH_Att,RSDWH_Att</v>
+      </c>
+      <c r="D67" s="32">
+        <f>AVERAGE(D27,D107)</f>
+        <v>3.5356636251858302E-2</v>
+      </c>
+      <c r="F67" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H67" s="32" t="str">
+        <f>"R-S*_"&amp;F67&amp;"_"&amp;G67&amp;"*"</f>
+        <v>R-S*_Att_SMF*</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B68" s="33" t="str">
+        <f t="shared" si="14"/>
+        <v>R-SW*Att_WOO*</v>
+      </c>
+      <c r="C68" s="33" t="str">
+        <f>"RSDSH_"&amp;F68&amp;",RSDWH_"&amp;F68</f>
+        <v>RSDSH_Att,RSDWH_Att</v>
+      </c>
+      <c r="D68" s="33">
+        <f>AVERAGE(D28,D108)</f>
+        <v>5.4484908352032999E-2</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H63" s="33" t="str">
-        <f>"R-S*_"&amp;F63&amp;"_"&amp;G63&amp;"*"</f>
+      <c r="H68" s="33" t="str">
+        <f>"R-S*_"&amp;F68&amp;"_"&amp;G68&amp;"*"</f>
         <v>R-S*_Att_WOO*</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="B64" s="32" t="str">
-        <f t="shared" si="16"/>
-        <v>R-SW*Att_HET*</v>
-      </c>
-      <c r="C64" s="32" t="str">
-        <f t="shared" si="15"/>
-        <v>RSDSH_Att,RSDWH_Att</v>
-      </c>
-      <c r="D64" s="32">
-        <f t="shared" si="13"/>
-        <v>9.6371031258262324E-3</v>
-      </c>
-      <c r="F64" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G64" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H64" s="32" t="str">
-        <f>"R-S*_"&amp;F64&amp;"_"&amp;G64&amp;"*"</f>
-        <v>R-S*_Att_HET*</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="30"/>
-    </row>
-    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="32" t="str">
-        <f>"R-SW*"&amp;F66&amp;"_"&amp;G66&amp;"*"</f>
-        <v>R-SW*Det_COA*</v>
-      </c>
-      <c r="C66" s="32" t="str">
-        <f>"RSDSH_"&amp;F66&amp;",RSDWH_"&amp;F66</f>
-        <v>RSDSH_Det,RSDWH_Det</v>
-      </c>
-      <c r="D66" s="32">
-        <f t="shared" ref="D66:D76" si="18">AVERAGE(D30,D104)</f>
-        <v>0.29527340147394254</v>
-      </c>
-      <c r="F66" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G66" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="H66" s="32" t="str">
-        <f t="shared" ref="H66:H70" si="19">"R-S*_"&amp;F66&amp;"_"&amp;G66&amp;"*"</f>
-        <v>R-S*_Det_COA*</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="33" t="str">
-        <f>"R-SW*"&amp;F67&amp;"_"&amp;G67&amp;"*"</f>
-        <v>R-SW*Det_BDL*</v>
-      </c>
-      <c r="C67" s="33" t="str">
-        <f t="shared" ref="C67:C76" si="20">"RSDSH_"&amp;F67&amp;",RSDWH_"&amp;F67</f>
-        <v>RSDSH_Det,RSDWH_Det</v>
-      </c>
-      <c r="D67" s="33">
-        <f t="shared" si="18"/>
-        <v>6.7726027397260503E-3</v>
-      </c>
-      <c r="F67" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G67" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H67" s="33" t="str">
-        <f t="shared" si="19"/>
-        <v>R-S*_Det_BDL*</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="32" t="str">
-        <f>"R-SW*"&amp;F68&amp;"_"&amp;G68&amp;"*"</f>
-        <v>R-SW*Det_ETH*</v>
-      </c>
-      <c r="C68" s="32" t="str">
-        <f t="shared" si="20"/>
-        <v>RSDSH_Det,RSDWH_Det</v>
-      </c>
-      <c r="D68" s="32">
-        <f t="shared" si="18"/>
-        <v>7.6715753424657501E-3</v>
-      </c>
-      <c r="F68" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G68" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H68" s="32" t="str">
-        <f t="shared" si="19"/>
-        <v>R-S*_Det_ETH*</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="B69" s="33" t="str">
-        <f>"R-SW*"&amp;F69&amp;"_"&amp;G69&amp;"*"</f>
-        <v>R-SW*Det_LPG*</v>
+      <c r="B69" s="33" t="s">
+        <v>271</v>
       </c>
       <c r="C69" s="33" t="str">
-        <f t="shared" si="20"/>
-        <v>RSDSH_Det,RSDWH_Det</v>
+        <f>"RSDSH_"&amp;F68&amp;",RSDWH_"&amp;F68</f>
+        <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D69" s="33">
-        <f t="shared" si="18"/>
-        <v>5.3518479911912255E-2</v>
-      </c>
-      <c r="F69" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G69" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="H69" s="33" t="str">
-        <f t="shared" si="19"/>
-        <v>R-S*_Det_LPG*</v>
-      </c>
+        <f>D68</f>
+        <v>5.4484908352032999E-2</v>
+      </c>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="33"/>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
         <v>198</v>
       </c>
       <c r="B70" s="32" t="str">
-        <f>"R-SW*"&amp;F70&amp;"_"&amp;G70&amp;"*"</f>
-        <v>R-SW*Det_ELC*</v>
+        <f t="shared" si="14"/>
+        <v>R-SW*Att_HET*</v>
       </c>
       <c r="C70" s="32" t="str">
-        <f t="shared" si="20"/>
-        <v>RSDSH_Det,RSDWH_Det</v>
+        <f t="shared" si="13"/>
+        <v>RSDSH_Att,RSDWH_Att</v>
       </c>
       <c r="D70" s="32">
-        <f t="shared" si="18"/>
-        <v>3.4771475539781452E-2</v>
+        <f>AVERAGE(D30,D109)</f>
+        <v>9.6371031258262324E-3</v>
       </c>
       <c r="F70" s="32" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="G70" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H70" s="32" t="str">
-        <f t="shared" si="19"/>
-        <v>R-S*_Det_ELC*</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B71" s="33" t="str">
-        <f t="shared" ref="B71:B76" si="21">"R-SW*"&amp;F71&amp;"_"&amp;G71&amp;"*"</f>
-        <v>R-SW*Det_KER*</v>
-      </c>
-      <c r="C71" s="33" t="str">
-        <f t="shared" si="20"/>
-        <v>RSDSH_Det,RSDWH_Det</v>
-      </c>
-      <c r="D71" s="33">
-        <f t="shared" si="18"/>
-        <v>3.8152557611937102E-2</v>
-      </c>
-      <c r="F71" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G71" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H71" s="33" t="str">
-        <f t="shared" ref="H71" si="22">"R-S*_"&amp;F71&amp;"_"&amp;G71&amp;"*"</f>
-        <v>R-S*_Det_KER*</v>
-      </c>
+        <f>"R-S*_"&amp;F70&amp;"_"&amp;G70&amp;"*"</f>
+        <v>R-S*_Att_HET*</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="32" t="s">
-        <v>198</v>
+        <v>1</v>
       </c>
       <c r="B72" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>R-SW*Det_GAS*</v>
+        <f>"R-SW*"&amp;F72&amp;"_"&amp;G72&amp;"*"</f>
+        <v>R-SW*Det_COA*</v>
       </c>
       <c r="C72" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f>"RSDSH_"&amp;F72&amp;",RSDWH_"&amp;F72</f>
         <v>RSDSH_Det,RSDWH_Det</v>
       </c>
       <c r="D72" s="32">
-        <f t="shared" si="18"/>
-        <v>3.1008650759600302E-2</v>
+        <f>AVERAGE(D32,D112)</f>
+        <v>0.29527340147394254</v>
       </c>
       <c r="F72" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G72" s="32" t="s">
-        <v>194</v>
+        <v>82</v>
       </c>
       <c r="H72" s="32" t="str">
-        <f>"R-S*_"&amp;F71&amp;"_"&amp;G72&amp;"*"</f>
-        <v>R-S*_Det_GAS*</v>
+        <f t="shared" ref="H72:H76" si="16">"R-S*_"&amp;F72&amp;"_"&amp;G72&amp;"*"</f>
+        <v>R-S*_Det_COA*</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7038,26 +6987,26 @@
         <v>1</v>
       </c>
       <c r="B73" s="33" t="str">
-        <f t="shared" si="21"/>
-        <v>R-SW*Det_PEA*</v>
+        <f>"R-SW*"&amp;F73&amp;"_"&amp;G73&amp;"*"</f>
+        <v>R-SW*Det_BDL*</v>
       </c>
       <c r="C73" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="C73:C84" si="17">"RSDSH_"&amp;F73&amp;",RSDWH_"&amp;F73</f>
         <v>RSDSH_Det,RSDWH_Det</v>
       </c>
       <c r="D73" s="33">
-        <f t="shared" si="18"/>
-        <v>6.8174234439631151E-2</v>
+        <f>AVERAGE(D33,D113)</f>
+        <v>6.7726027397260503E-3</v>
       </c>
       <c r="F73" s="33" t="s">
         <v>114</v>
       </c>
       <c r="G73" s="33" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="H73" s="33" t="str">
-        <f>"R-S*_"&amp;F73&amp;"_"&amp;G73&amp;"*"</f>
-        <v>R-S*_Det_PEA*</v>
+        <f t="shared" si="16"/>
+        <v>R-S*_Det_BDL*</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7065,26 +7014,26 @@
         <v>1</v>
       </c>
       <c r="B74" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>R-SW*Det_SMF*</v>
+        <f>"R-SW*"&amp;F74&amp;"_"&amp;G74&amp;"*"</f>
+        <v>R-SW*Det_ETH*</v>
       </c>
       <c r="C74" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>RSDSH_Det,RSDWH_Det</v>
       </c>
       <c r="D74" s="32">
-        <f t="shared" si="18"/>
-        <v>8.9483268751498007E-2</v>
+        <f>AVERAGE(D34,D114)</f>
+        <v>7.6715753424657501E-3</v>
       </c>
       <c r="F74" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G74" s="32" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="H74" s="32" t="str">
-        <f>"R-S*_"&amp;F74&amp;"_"&amp;G74&amp;"*"</f>
-        <v>R-S*_Det_SMF*</v>
+        <f t="shared" si="16"/>
+        <v>R-S*_Det_ETH*</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7092,26 +7041,26 @@
         <v>198</v>
       </c>
       <c r="B75" s="33" t="str">
-        <f t="shared" si="21"/>
-        <v>R-SW*Det_WOO*</v>
+        <f>"R-SW*"&amp;F75&amp;"_"&amp;G75&amp;"*"</f>
+        <v>R-SW*Det_LPG*</v>
       </c>
       <c r="C75" s="33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>RSDSH_Det,RSDWH_Det</v>
       </c>
       <c r="D75" s="33">
-        <f t="shared" si="18"/>
-        <v>6.705720075762131E-2</v>
+        <f>AVERAGE(D35,D115)</f>
+        <v>5.3518479911912255E-2</v>
       </c>
       <c r="F75" s="33" t="s">
         <v>114</v>
       </c>
       <c r="G75" s="33" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H75" s="33" t="str">
-        <f>"R-S*_"&amp;F75&amp;"_"&amp;G75&amp;"*"</f>
-        <v>R-S*_Det_WOO*</v>
+        <f t="shared" si="16"/>
+        <v>R-S*_Det_LPG*</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7119,253 +7068,261 @@
         <v>198</v>
       </c>
       <c r="B76" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>R-SW*Det_HET*</v>
+        <f>"R-SW*"&amp;F76&amp;"_"&amp;G76&amp;"*"</f>
+        <v>R-SW*Det_ELC*</v>
       </c>
       <c r="C76" s="32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>RSDSH_Det,RSDWH_Det</v>
       </c>
       <c r="D76" s="32">
-        <f t="shared" si="18"/>
-        <v>0.12131157231005595</v>
+        <f>AVERAGE(D36,D116)</f>
+        <v>3.4771475539781452E-2</v>
       </c>
       <c r="F76" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G76" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H76" s="32" t="str">
-        <f>"R-S*_"&amp;F76&amp;"_"&amp;G76&amp;"*"</f>
-        <v>R-S*_Det_HET*</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="31"/>
-      <c r="F77" s="30"/>
-      <c r="G77" s="30"/>
-      <c r="H77" s="30"/>
+        <f t="shared" si="16"/>
+        <v>R-S*_Det_ELC*</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B77" s="33" t="str">
+        <f t="shared" ref="B77:B84" si="18">"R-SW*"&amp;F77&amp;"_"&amp;G77&amp;"*"</f>
+        <v>R-SW*Det_KER*</v>
+      </c>
+      <c r="C77" s="33" t="str">
+        <f t="shared" si="17"/>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
+      <c r="D77" s="33">
+        <f>AVERAGE(D37,D117)</f>
+        <v>3.8152557611937102E-2</v>
+      </c>
+      <c r="F77" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G77" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H77" s="33" t="str">
+        <f t="shared" ref="H77" si="19">"R-S*_"&amp;F77&amp;"_"&amp;G77&amp;"*"</f>
+        <v>R-S*_Det_KER*</v>
+      </c>
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B78" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="C78" s="33" t="str">
+        <f>"RSDSH_"&amp;F77&amp;",RSDWH_"&amp;F77</f>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
+      <c r="D78" s="33">
+        <f>D77</f>
+        <v>3.8152557611937102E-2</v>
+      </c>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="33"/>
+    </row>
+    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79" s="32" t="str">
+        <f t="shared" si="18"/>
+        <v>R-SW*Det_GAS*</v>
+      </c>
+      <c r="C79" s="32" t="str">
+        <f t="shared" si="17"/>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
+      <c r="D79" s="32">
+        <f>AVERAGE(D39,D118)</f>
+        <v>3.1008650759600302E-2</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G79" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="H79" s="32" t="str">
+        <f>"R-S*_"&amp;F77&amp;"_"&amp;G79&amp;"*"</f>
+        <v>R-S*_Det_GAS*</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B78" s="32" t="str">
-        <f t="shared" ref="B78:B88" si="23">"R-WH_"&amp;F78&amp;"_"&amp;G78&amp;"*"</f>
-        <v>R-WH_Apt_COA*</v>
-      </c>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H78,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>5.4306956259161203E-2</v>
-      </c>
-      <c r="F78" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G78" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="H78" s="32" t="str">
-        <f t="shared" ref="H78:H83" si="24">"R-WH_"&amp;F78&amp;"_"&amp;G78&amp;"*"</f>
-        <v>R-WH_Apt_COA*</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="33" t="s">
+      <c r="B80" s="33" t="str">
+        <f t="shared" si="18"/>
+        <v>R-SW*Det_PEA*</v>
+      </c>
+      <c r="C80" s="33" t="str">
+        <f t="shared" si="17"/>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
+      <c r="D80" s="33">
+        <f>AVERAGE(D40,D119)</f>
+        <v>6.8174234439631151E-2</v>
+      </c>
+      <c r="F80" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G80" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H80" s="33" t="str">
+        <f>"R-S*_"&amp;F80&amp;"_"&amp;G80&amp;"*"</f>
+        <v>R-S*_Det_PEA*</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="33" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_BDL*</v>
-      </c>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H79,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>9.0061643835616396E-3</v>
-      </c>
-      <c r="F79" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G79" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H79" s="33" t="str">
-        <f t="shared" si="24"/>
-        <v>R-WH_Apt_BDL*</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="32" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_ETH*</v>
-      </c>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H80,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.08506849315068E-2</v>
-      </c>
-      <c r="F80" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G80" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H80" s="32" t="str">
-        <f t="shared" si="24"/>
-        <v>R-WH_Apt_ETH*</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B81" s="33" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_LPG*</v>
-      </c>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H81,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.5902117368476298E-2</v>
-      </c>
-      <c r="F81" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G81" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="H81" s="33" t="str">
-        <f t="shared" si="24"/>
-        <v>R-WH_Apt_LPG*</v>
+      <c r="B81" s="32" t="str">
+        <f t="shared" si="18"/>
+        <v>R-SW*Det_SMF*</v>
+      </c>
+      <c r="C81" s="32" t="str">
+        <f t="shared" si="17"/>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
+      <c r="D81" s="32">
+        <f>AVERAGE(D41,D120)</f>
+        <v>8.9483268751498007E-2</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G81" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H81" s="32" t="str">
+        <f>"R-S*_"&amp;F81&amp;"_"&amp;G81&amp;"*"</f>
+        <v>R-S*_Det_SMF*</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B82" s="32" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_ELC*</v>
-      </c>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H82,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.8837772266824751E-2</v>
-      </c>
-      <c r="F82" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G82" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H82" s="32" t="str">
-        <f>B82</f>
-        <v>R-WH_Apt_ELC*</v>
+      <c r="A82" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B82" s="33" t="str">
+        <f t="shared" si="18"/>
+        <v>R-SW*Det_WOO*</v>
+      </c>
+      <c r="C82" s="33" t="str">
+        <f t="shared" si="17"/>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
+      <c r="D82" s="33">
+        <f>AVERAGE(D42,D121)</f>
+        <v>6.705720075762131E-2</v>
+      </c>
+      <c r="F82" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G82" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H82" s="33" t="str">
+        <f>"R-S*_"&amp;F82&amp;"_"&amp;G82&amp;"*"</f>
+        <v>R-S*_Det_WOO*</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B83" s="33" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_KER*</v>
-      </c>
-      <c r="C83" s="33"/>
+        <v>198</v>
+      </c>
+      <c r="B83" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C83" s="33" t="str">
+        <f>"RSDSH_"&amp;F82&amp;",RSDWH_"&amp;F82</f>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
       <c r="D83" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H83,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.34604040212748E-2</v>
-      </c>
-      <c r="F83" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G83" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H83" s="33" t="str">
-        <f t="shared" si="24"/>
-        <v>R-WH_Apt_KER*</v>
-      </c>
+        <f>D82</f>
+        <v>6.705720075762131E-2</v>
+      </c>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="32" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B84" s="32" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_GAS*</v>
-      </c>
-      <c r="C84" s="32"/>
+        <f t="shared" si="18"/>
+        <v>R-SW*Det_HET*</v>
+      </c>
+      <c r="C84" s="32" t="str">
+        <f t="shared" si="17"/>
+        <v>RSDSH_Det,RSDWH_Det</v>
+      </c>
       <c r="D84" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H84,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>9.0054738416460393E-3</v>
+        <f>AVERAGE(D44,D122)</f>
+        <v>0.12131157231005595</v>
       </c>
       <c r="F84" s="32" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G84" s="32" t="s">
-        <v>194</v>
+        <v>84</v>
       </c>
       <c r="H84" s="32" t="str">
-        <f>"R-WH_"&amp;F83&amp;"_"&amp;G84&amp;"*"</f>
-        <v>R-WH_Apt_GAS*</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85" s="33" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_PEA*</v>
-      </c>
-      <c r="C85" s="33"/>
-      <c r="D85" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H85,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.0875263435194901E-2</v>
-      </c>
-      <c r="F85" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G85" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="H85" s="33" t="str">
-        <f t="shared" ref="H85:H89" si="25">"R-WH_"&amp;F85&amp;"_"&amp;G85&amp;"*"</f>
-        <v>R-WH_Apt_PEA*</v>
-      </c>
+        <f>"R-S*_"&amp;F84&amp;"_"&amp;G84&amp;"*"</f>
+        <v>R-S*_Det_HET*</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A85" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="31"/>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30"/>
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="32" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_SMF*</v>
+        <f t="shared" ref="B86:B96" si="20">"R-WH_"&amp;F86&amp;"_"&amp;G86&amp;"*"</f>
+        <v>R-WH_Apt_COA*</v>
       </c>
       <c r="C86" s="32"/>
       <c r="D86" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H86,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.0823557576601301E-2</v>
+        <v>5.4306956259161203E-2</v>
       </c>
       <c r="F86" s="32" t="s">
         <v>109</v>
       </c>
       <c r="G86" s="32" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="H86" s="32" t="str">
-        <f t="shared" si="25"/>
-        <v>R-WH_Apt_SMF*</v>
+        <f t="shared" ref="H86:H91" si="21">"R-WH_"&amp;F86&amp;"_"&amp;G86&amp;"*"</f>
+        <v>R-WH_Apt_COA*</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7373,23 +7330,23 @@
         <v>1</v>
       </c>
       <c r="B87" s="33" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_WOO*</v>
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_BDL*</v>
       </c>
       <c r="C87" s="33"/>
       <c r="D87" s="33">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H87,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.23793448122469E-2</v>
+        <v>9.0061643835616396E-3</v>
       </c>
       <c r="F87" s="33" t="s">
         <v>109</v>
       </c>
       <c r="G87" s="33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H87" s="33" t="str">
-        <f t="shared" si="25"/>
-        <v>R-WH_Apt_WOO*</v>
+        <f t="shared" si="21"/>
+        <v>R-WH_Apt_BDL*</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7397,275 +7354,275 @@
         <v>1</v>
       </c>
       <c r="B88" s="32" t="str">
-        <f t="shared" si="23"/>
-        <v>R-WH_Apt_HET*</v>
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_ETH*</v>
       </c>
       <c r="C88" s="32"/>
       <c r="D88" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H88,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>3.8847834889027099E-4</v>
+        <v>1.08506849315068E-2</v>
       </c>
       <c r="F88" s="32" t="s">
         <v>109</v>
       </c>
       <c r="G88" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="H88" s="32" t="str">
+        <f t="shared" si="21"/>
+        <v>R-WH_Apt_ETH*</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="33" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_LPG*</v>
+      </c>
+      <c r="C89" s="33"/>
+      <c r="D89" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H89,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.5902117368476298E-2</v>
+      </c>
+      <c r="F89" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G89" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="H89" s="33" t="str">
+        <f t="shared" si="21"/>
+        <v>R-WH_Apt_LPG*</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B90" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_ELC*</v>
+      </c>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H90,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.8837772266824751E-2</v>
+      </c>
+      <c r="F90" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G90" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H90" s="32" t="str">
+        <f>B90</f>
+        <v>R-WH_Apt_ELC*</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="33" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_KER*</v>
+      </c>
+      <c r="C91" s="33"/>
+      <c r="D91" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H91,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.34604040212748E-2</v>
+      </c>
+      <c r="F91" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G91" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H91" s="33" t="str">
+        <f t="shared" si="21"/>
+        <v>R-WH_Apt_KER*</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_GAS*</v>
+      </c>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H92,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>9.0054738416460393E-3</v>
+      </c>
+      <c r="F92" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G92" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="H92" s="32" t="str">
+        <f>"R-WH_"&amp;F91&amp;"_"&amp;G92&amp;"*"</f>
+        <v>R-WH_Apt_GAS*</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="33" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_PEA*</v>
+      </c>
+      <c r="C93" s="33"/>
+      <c r="D93" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H93,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.0875263435194901E-2</v>
+      </c>
+      <c r="F93" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G93" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H93" s="33" t="str">
+        <f t="shared" ref="H93:H97" si="22">"R-WH_"&amp;F93&amp;"_"&amp;G93&amp;"*"</f>
+        <v>R-WH_Apt_PEA*</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_SMF*</v>
+      </c>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H94,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.0823557576601301E-2</v>
+      </c>
+      <c r="F94" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G94" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H94" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>R-WH_Apt_SMF*</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="33" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_WOO*</v>
+      </c>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H95,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.23793448122469E-2</v>
+      </c>
+      <c r="F95" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G95" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H95" s="33" t="str">
+        <f t="shared" si="22"/>
+        <v>R-WH_Apt_WOO*</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>R-WH_Apt_HET*</v>
+      </c>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H96,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>3.8847834889027099E-4</v>
+      </c>
+      <c r="F96" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G96" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H88" s="32" t="str">
-        <f t="shared" si="25"/>
+      <c r="H96" s="32" t="str">
+        <f t="shared" si="22"/>
         <v>R-WH_Apt_HET*</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B89" s="32" t="str">
-        <f>"R-WH_"&amp;F89&amp;"_"&amp;G89&amp;"*"</f>
-        <v>R-WH_Apt_SOL*</v>
-      </c>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H89,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.0946059106357601E-2</v>
-      </c>
-      <c r="F89" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G89" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="H89" s="32" t="str">
-        <f t="shared" si="25"/>
-        <v>R-WH_Apt_SOL*</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-    </row>
-    <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" s="32" t="str">
-        <f t="shared" ref="B91:B101" si="26">"R-WH_"&amp;F91&amp;"_"&amp;G91&amp;"*"</f>
-        <v>R-WH_Att_COA*</v>
-      </c>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H91,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.0871971515326802E-2</v>
-      </c>
-      <c r="F91" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G91" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="H91" s="32" t="str">
-        <f t="shared" ref="H91:H96" si="27">"R-WH_"&amp;F91&amp;"_"&amp;G91&amp;"*"</f>
-        <v>R-WH_Att_COA*</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B92" s="33" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_BDL*</v>
-      </c>
-      <c r="C92" s="33"/>
-      <c r="D92" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H92,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.7783866057838701E-2</v>
-      </c>
-      <c r="F92" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G92" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H92" s="33" t="str">
-        <f t="shared" si="27"/>
-        <v>R-WH_Att_BDL*</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B93" s="32" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_ETH*</v>
-      </c>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H93,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.34424657534247E-2</v>
-      </c>
-      <c r="F93" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G93" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H93" s="32" t="str">
-        <f t="shared" si="27"/>
-        <v>R-WH_Att_ETH*</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B94" s="33" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_LPG*</v>
-      </c>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H94,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.01134837356341E-2</v>
-      </c>
-      <c r="F94" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G94" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="H94" s="33" t="str">
-        <f t="shared" si="27"/>
-        <v>R-WH_Att_LPG*</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B95" s="32" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_ELC*</v>
-      </c>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H95,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.6397220281969702E-2</v>
-      </c>
-      <c r="F95" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G95" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H95" s="32" t="str">
-        <f>"R-WH_"&amp;F95&amp;"_"&amp;G95&amp;"*X0"</f>
-        <v>R-WH_Att_ELC*X0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B96" s="33" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_KER*</v>
-      </c>
-      <c r="C96" s="33"/>
-      <c r="D96" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H96,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.39410555733958E-2</v>
-      </c>
-      <c r="F96" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G96" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H96" s="33" t="str">
-        <f t="shared" si="27"/>
-        <v>R-WH_Att_KER*</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="32" t="s">
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="B97" s="32" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_GAS*</v>
+        <f>"R-WH_"&amp;F97&amp;"_"&amp;G97&amp;"*"</f>
+        <v>R-WH_Apt_SOL*</v>
       </c>
       <c r="C97" s="32"/>
       <c r="D97" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H97,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.16777135974941E-2</v>
+        <v>1.0946059106357601E-2</v>
       </c>
       <c r="F97" s="32" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G97" s="32" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="H97" s="32" t="str">
-        <f>"R-WH_"&amp;F96&amp;"_"&amp;G97&amp;"*"</f>
-        <v>R-WH_Att_GAS*</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="33" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_PEA*</v>
-      </c>
-      <c r="C98" s="33"/>
-      <c r="D98" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H98,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.3788861785020401E-2</v>
-      </c>
-      <c r="F98" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G98" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="H98" s="33" t="str">
-        <f t="shared" ref="H98:H102" si="28">"R-WH_"&amp;F98&amp;"_"&amp;G98&amp;"*"</f>
-        <v>R-WH_Att_PEA*</v>
-      </c>
+        <f t="shared" si="22"/>
+        <v>R-WH_Apt_SOL*</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A98" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="30"/>
+      <c r="F98" s="30"/>
+      <c r="G98" s="30"/>
+      <c r="H98" s="30"/>
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B99" s="32" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_SMF*</v>
+        <f t="shared" ref="B99:B109" si="23">"R-WH_"&amp;F99&amp;"_"&amp;G99&amp;"*"</f>
+        <v>R-WH_Att_COA*</v>
       </c>
       <c r="C99" s="32"/>
       <c r="D99" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H99,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.1808127750471799E-2</v>
+        <v>2.0871971515326802E-2</v>
       </c>
       <c r="F99" s="32" t="s">
         <v>105</v>
       </c>
       <c r="G99" s="32" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="H99" s="32" t="str">
-        <f t="shared" si="28"/>
-        <v>R-WH_Att_SMF*</v>
+        <f t="shared" ref="H99:H104" si="24">"R-WH_"&amp;F99&amp;"_"&amp;G99&amp;"*"</f>
+        <v>R-WH_Att_COA*</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7673,23 +7630,23 @@
         <v>1</v>
       </c>
       <c r="B100" s="33" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_WOO*</v>
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_BDL*</v>
       </c>
       <c r="C100" s="33"/>
       <c r="D100" s="33">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H100,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.3755627925516699E-2</v>
+        <v>1.7783866057838701E-2</v>
       </c>
       <c r="F100" s="33" t="s">
         <v>105</v>
       </c>
       <c r="G100" s="33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H100" s="33" t="str">
-        <f t="shared" si="28"/>
-        <v>R-WH_Att_WOO*</v>
+        <f t="shared" si="24"/>
+        <v>R-WH_Att_BDL*</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7697,275 +7654,275 @@
         <v>1</v>
       </c>
       <c r="B101" s="32" t="str">
-        <f t="shared" si="26"/>
-        <v>R-WH_Att_HET*</v>
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_ETH*</v>
       </c>
       <c r="C101" s="32"/>
       <c r="D101" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H101,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>9.7589168523886695E-4</v>
+        <v>1.34424657534247E-2</v>
       </c>
       <c r="F101" s="32" t="s">
         <v>105</v>
       </c>
       <c r="G101" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="H101" s="32" t="str">
+        <f t="shared" si="24"/>
+        <v>R-WH_Att_ETH*</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="33" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_LPG*</v>
+      </c>
+      <c r="C102" s="33"/>
+      <c r="D102" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H102,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.01134837356341E-2</v>
+      </c>
+      <c r="F102" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G102" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="H102" s="33" t="str">
+        <f t="shared" si="24"/>
+        <v>R-WH_Att_LPG*</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_ELC*</v>
+      </c>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H103,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.6397220281969702E-2</v>
+      </c>
+      <c r="F103" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G103" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H103" s="32" t="str">
+        <f>"R-WH_"&amp;F103&amp;"_"&amp;G103&amp;"*X0"</f>
+        <v>R-WH_Att_ELC*X0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B104" s="33" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_KER*</v>
+      </c>
+      <c r="C104" s="33"/>
+      <c r="D104" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H104,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.39410555733958E-2</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G104" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H104" s="33" t="str">
+        <f t="shared" si="24"/>
+        <v>R-WH_Att_KER*</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_GAS*</v>
+      </c>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H105,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.16777135974941E-2</v>
+      </c>
+      <c r="F105" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G105" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="H105" s="32" t="str">
+        <f>"R-WH_"&amp;F104&amp;"_"&amp;G105&amp;"*"</f>
+        <v>R-WH_Att_GAS*</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="33" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_PEA*</v>
+      </c>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H106,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.3788861785020401E-2</v>
+      </c>
+      <c r="F106" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G106" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H106" s="33" t="str">
+        <f t="shared" ref="H106:H110" si="25">"R-WH_"&amp;F106&amp;"_"&amp;G106&amp;"*"</f>
+        <v>R-WH_Att_PEA*</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_SMF*</v>
+      </c>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H107,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.1808127750471799E-2</v>
+      </c>
+      <c r="F107" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G107" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H107" s="32" t="str">
+        <f t="shared" si="25"/>
+        <v>R-WH_Att_SMF*</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="33" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_WOO*</v>
+      </c>
+      <c r="C108" s="33"/>
+      <c r="D108" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H108,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.3755627925516699E-2</v>
+      </c>
+      <c r="F108" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G108" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H108" s="33" t="str">
+        <f t="shared" si="25"/>
+        <v>R-WH_Att_WOO*</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>R-WH_Att_HET*</v>
+      </c>
+      <c r="C109" s="32"/>
+      <c r="D109" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H109,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>9.7589168523886695E-4</v>
+      </c>
+      <c r="F109" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G109" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H101" s="32" t="str">
-        <f t="shared" si="28"/>
+      <c r="H109" s="32" t="str">
+        <f t="shared" si="25"/>
         <v>R-WH_Att_HET*</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B102" s="32" t="str">
-        <f>"R-WH_"&amp;F102&amp;"_"&amp;G102&amp;"*"</f>
-        <v>R-WH_Att_SOL*</v>
-      </c>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H102,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>4.36448583018159E-2</v>
-      </c>
-      <c r="F102" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G102" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="H102" s="32" t="str">
-        <f t="shared" si="28"/>
-        <v>R-WH_Att_SOL*</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A103" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B103" s="30"/>
-      <c r="C103" s="30"/>
-      <c r="D103" s="30"/>
-      <c r="E103" s="30"/>
-      <c r="F103" s="30"/>
-      <c r="G103" s="30"/>
-      <c r="H103" s="30"/>
-    </row>
-    <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B104" s="32" t="str">
-        <f t="shared" ref="B104:B114" si="29">"R-WH_"&amp;F104&amp;"_"&amp;G104&amp;"*"</f>
-        <v>R-WH_Det_COA*</v>
-      </c>
-      <c r="C104" s="32"/>
-      <c r="D104" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H104,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.3205860842012E-2</v>
-      </c>
-      <c r="F104" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G104" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="H104" s="32" t="str">
-        <f t="shared" ref="H104:H109" si="30">"R-WH_"&amp;F104&amp;"_"&amp;G104&amp;"*"</f>
-        <v>R-WH_Det_COA*</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B105" s="33" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_BDL*</v>
-      </c>
-      <c r="C105" s="33"/>
-      <c r="D105" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H105,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.3545205479452101E-2</v>
-      </c>
-      <c r="F105" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G105" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H105" s="33" t="str">
-        <f t="shared" si="30"/>
-        <v>R-WH_Det_BDL*</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B106" s="32" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_ETH*</v>
-      </c>
-      <c r="C106" s="32"/>
-      <c r="D106" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H106,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.53431506849315E-2</v>
-      </c>
-      <c r="F106" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G106" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H106" s="32" t="str">
-        <f t="shared" si="30"/>
-        <v>R-WH_Det_ETH*</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B107" s="33" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_LPG*</v>
-      </c>
-      <c r="C107" s="33"/>
-      <c r="D107" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H107,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.20120031139646E-2</v>
-      </c>
-      <c r="F107" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G107" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="H107" s="33" t="str">
-        <f t="shared" si="30"/>
-        <v>R-WH_Det_LPG*</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B108" s="32" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_ELC*</v>
-      </c>
-      <c r="C108" s="32"/>
-      <c r="D108" s="32">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H108,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.6905741708612799E-2</v>
-      </c>
-      <c r="F108" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G108" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H108" s="32" t="str">
-        <f>"R-WH_"&amp;F108&amp;"_"&amp;G108&amp;"*X0"</f>
-        <v>R-WH_Det_ELC*X0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B109" s="33" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_KER*</v>
-      </c>
-      <c r="C109" s="33"/>
-      <c r="D109" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H109,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.71705033816347E-2</v>
-      </c>
-      <c r="F109" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G109" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H109" s="33" t="str">
-        <f t="shared" si="30"/>
-        <v>R-WH_Det_KER*</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="32" t="s">
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="B110" s="32" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_GAS*</v>
+        <f>"R-WH_"&amp;F110&amp;"_"&amp;G110&amp;"*"</f>
+        <v>R-WH_Att_SOL*</v>
       </c>
       <c r="C110" s="32"/>
       <c r="D110" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H110,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.5035273157845299E-2</v>
+        <v>4.36448583018159E-2</v>
       </c>
       <c r="F110" s="32" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="G110" s="32" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="H110" s="32" t="str">
-        <f>"R-WH_"&amp;F109&amp;"_"&amp;G110&amp;"*"</f>
-        <v>R-WH_Det_GAS*</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B111" s="33" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_PEA*</v>
-      </c>
-      <c r="C111" s="33"/>
-      <c r="D111" s="33">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H111,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.5844216359380301E-2</v>
-      </c>
-      <c r="F111" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G111" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="H111" s="33" t="str">
-        <f t="shared" ref="H111:H115" si="31">"R-WH_"&amp;F111&amp;"_"&amp;G111&amp;"*"</f>
-        <v>R-WH_Det_PEA*</v>
-      </c>
+        <f t="shared" si="25"/>
+        <v>R-WH_Att_SOL*</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A111" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B111" s="30"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="30"/>
+      <c r="F111" s="30"/>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
     </row>
     <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B112" s="32" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_SMF*</v>
+        <f t="shared" ref="B112:B122" si="26">"R-WH_"&amp;F112&amp;"_"&amp;G112&amp;"*"</f>
+        <v>R-WH_Det_COA*</v>
       </c>
       <c r="C112" s="32"/>
       <c r="D112" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H112,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.4316024530344E-2</v>
+        <v>2.3205860842012E-2</v>
       </c>
       <c r="F112" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G112" s="32" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="H112" s="32" t="str">
-        <f t="shared" si="31"/>
-        <v>R-WH_Det_SMF*</v>
+        <f t="shared" ref="H112:H117" si="27">"R-WH_"&amp;F112&amp;"_"&amp;G112&amp;"*"</f>
+        <v>R-WH_Det_COA*</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7973,23 +7930,23 @@
         <v>1</v>
       </c>
       <c r="B113" s="33" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_WOO*</v>
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_BDL*</v>
       </c>
       <c r="C113" s="33"/>
       <c r="D113" s="33">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H113,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.8495641261436602E-2</v>
+        <v>1.3545205479452101E-2</v>
       </c>
       <c r="F113" s="33" t="s">
         <v>114</v>
       </c>
       <c r="G113" s="33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H113" s="33" t="str">
-        <f t="shared" si="31"/>
-        <v>R-WH_Det_WOO*</v>
+        <f t="shared" si="27"/>
+        <v>R-WH_Det_BDL*</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7997,229 +7954,244 @@
         <v>1</v>
       </c>
       <c r="B114" s="32" t="str">
-        <f t="shared" si="29"/>
-        <v>R-WH_Det_HET*</v>
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_ETH*</v>
       </c>
       <c r="C114" s="32"/>
       <c r="D114" s="32">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H114,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>1.6330345396658901E-3</v>
+        <v>1.53431506849315E-2</v>
       </c>
       <c r="F114" s="32" t="s">
         <v>114</v>
       </c>
       <c r="G114" s="32" t="s">
-        <v>84</v>
+        <v>190</v>
       </c>
       <c r="H114" s="32" t="str">
-        <f t="shared" si="31"/>
-        <v>R-WH_Det_HET*</v>
+        <f t="shared" si="27"/>
+        <v>R-WH_Det_ETH*</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="32" t="s">
+      <c r="A115" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B115" s="33" t="str">
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_LPG*</v>
+      </c>
+      <c r="C115" s="33"/>
+      <c r="D115" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H115,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.20120031139646E-2</v>
+      </c>
+      <c r="F115" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G115" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="H115" s="33" t="str">
+        <f t="shared" si="27"/>
+        <v>R-WH_Det_LPG*</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="B115" s="32" t="str">
-        <f>"R-WH_"&amp;F115&amp;"_"&amp;G115&amp;"*"</f>
-        <v>R-WH_Det_SOL*</v>
-      </c>
-      <c r="C115" s="32"/>
-      <c r="D115" s="40">
-        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H115,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>4.6408942067286699E-2</v>
-      </c>
-      <c r="F115" s="32" t="s">
+      <c r="B116" s="32" t="str">
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_ELC*</v>
+      </c>
+      <c r="C116" s="32"/>
+      <c r="D116" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H116,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.6905741708612799E-2</v>
+      </c>
+      <c r="F116" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="G115" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="H115" s="32" t="str">
-        <f t="shared" si="31"/>
-        <v>R-WH_Det_SOL*</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A116" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="B116" s="30"/>
-      <c r="C116" s="31"/>
-      <c r="D116" s="30"/>
-      <c r="E116" s="30"/>
-      <c r="F116" s="30"/>
-      <c r="G116" s="30"/>
-      <c r="H116" s="30"/>
+      <c r="G116" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H116" s="32" t="str">
+        <f>"R-WH_"&amp;F116&amp;"_"&amp;G116&amp;"*X0"</f>
+        <v>R-WH_Det_ELC*X0</v>
+      </c>
     </row>
     <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B117" s="32" t="str">
-        <f>"R-SC_"&amp;F117&amp;"_"&amp;G117&amp;"_N1"</f>
-        <v>R-SC_Apt_ELC_N1</v>
-      </c>
-      <c r="C117" s="32"/>
-      <c r="D117" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H117,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.6752418704136399E-2</v>
-      </c>
-      <c r="F117" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G117" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H117" s="37" t="str">
-        <f t="shared" ref="H117:H119" si="32">"R-SH_"&amp;F117&amp;"_"&amp;G117&amp;"*X1"</f>
-        <v>R-SH_Apt_ELC*X1</v>
+      <c r="A117" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B117" s="33" t="str">
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_KER*</v>
+      </c>
+      <c r="C117" s="33"/>
+      <c r="D117" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H117,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.71705033816347E-2</v>
+      </c>
+      <c r="F117" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G117" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H117" s="33" t="str">
+        <f t="shared" si="27"/>
+        <v>R-WH_Det_KER*</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="32" t="s">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="B118" s="32" t="str">
-        <f>"R-SC_"&amp;F118&amp;"_"&amp;G118&amp;"_N1"</f>
-        <v>R-SC_Att_ELC_N1</v>
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_GAS*</v>
       </c>
       <c r="C118" s="32"/>
       <c r="D118" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H118,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.1795378605209401E-2</v>
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H118,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.5035273157845299E-2</v>
       </c>
       <c r="F118" s="32" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G118" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H118" s="37" t="str">
-        <f t="shared" si="32"/>
-        <v>R-SH_Att_ELC*X1</v>
+        <v>194</v>
+      </c>
+      <c r="H118" s="32" t="str">
+        <f>"R-WH_"&amp;F117&amp;"_"&amp;G118&amp;"*"</f>
+        <v>R-WH_Det_GAS*</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B119" s="32" t="str">
-        <f>"R-SC_"&amp;F119&amp;"_"&amp;G119&amp;"_N1"</f>
-        <v>R-SC_Det_ELC_N1</v>
-      </c>
-      <c r="C119" s="32"/>
-      <c r="D119" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H119,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>4.0026061338975703E-2</v>
-      </c>
-      <c r="F119" s="32" t="s">
+      <c r="A119" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="33" t="str">
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_PEA*</v>
+      </c>
+      <c r="C119" s="33"/>
+      <c r="D119" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H119,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.5844216359380301E-2</v>
+      </c>
+      <c r="F119" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="G119" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H119" s="37" t="str">
-        <f t="shared" si="32"/>
-        <v>R-SH_Det_ELC*X1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A120" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="B120" s="30"/>
-      <c r="C120" s="31"/>
-      <c r="D120" s="30"/>
-      <c r="E120" s="30"/>
-      <c r="F120" s="30"/>
-      <c r="G120" s="30"/>
-      <c r="H120" s="30"/>
+      <c r="G119" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H119" s="33" t="str">
+        <f t="shared" ref="H119:H123" si="28">"R-WH_"&amp;F119&amp;"_"&amp;G119&amp;"*"</f>
+        <v>R-WH_Det_PEA*</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="32" t="str">
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_SMF*</v>
+      </c>
+      <c r="C120" s="32"/>
+      <c r="D120" s="32">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H120,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.4316024530344E-2</v>
+      </c>
+      <c r="F120" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G120" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H120" s="32" t="str">
+        <f t="shared" si="28"/>
+        <v>R-WH_Det_SMF*</v>
+      </c>
     </row>
     <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="B121" s="32" t="str">
-        <f>"R-HC_"&amp;F121&amp;"_"&amp;G121&amp;"_HPN*"</f>
-        <v>R-HC_Apt_ELC_HPN*</v>
-      </c>
-      <c r="C121" s="32" t="str">
-        <f>"RSDSC_"&amp;F121</f>
-        <v>RSDSC_Apt</v>
-      </c>
-      <c r="D121" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H121,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.6752418704136399E-2</v>
-      </c>
-      <c r="F121" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G121" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H121" s="37" t="str">
-        <f t="shared" ref="H121:H123" si="33">"R-SH_"&amp;F121&amp;"_"&amp;G121&amp;"*X1"</f>
-        <v>R-SH_Apt_ELC*X1</v>
+      <c r="A121" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B121" s="33" t="str">
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_WOO*</v>
+      </c>
+      <c r="C121" s="33"/>
+      <c r="D121" s="33">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H121,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.8495641261436602E-2</v>
+      </c>
+      <c r="F121" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G121" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H121" s="33" t="str">
+        <f t="shared" si="28"/>
+        <v>R-WH_Det_WOO*</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="32" t="s">
-        <v>245</v>
+        <v>1</v>
       </c>
       <c r="B122" s="32" t="str">
-        <f>"R-HC_"&amp;F122&amp;"_"&amp;G122&amp;"_HPN*"</f>
-        <v>R-HC_Att_ELC_HPN*</v>
-      </c>
-      <c r="C122" s="32" t="str">
-        <f>"RSDSC_"&amp;F122</f>
-        <v>RSDSC_Att</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>R-WH_Det_HET*</v>
+      </c>
+      <c r="C122" s="32"/>
       <c r="D122" s="32">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H122,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.1795378605209401E-2</v>
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H122,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>1.6330345396658901E-3</v>
       </c>
       <c r="F122" s="32" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G122" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H122" s="37" t="str">
-        <f t="shared" si="33"/>
-        <v>R-SH_Att_ELC*X1</v>
+        <v>84</v>
+      </c>
+      <c r="H122" s="32" t="str">
+        <f t="shared" si="28"/>
+        <v>R-WH_Det_HET*</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A123" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="B123" s="38" t="str">
-        <f>"R-HC_"&amp;F123&amp;"_"&amp;G123&amp;"_HPN*"</f>
-        <v>R-HC_Det_ELC_HPN*</v>
-      </c>
-      <c r="C123" s="38" t="str">
-        <f>"RSDSC_"&amp;F123</f>
-        <v>RSDSC_Det</v>
-      </c>
-      <c r="D123" s="38">
-        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H123,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>4.0026061338975703E-2</v>
-      </c>
-      <c r="F123" s="38" t="s">
+      <c r="A123" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="32" t="str">
+        <f>"R-WH_"&amp;F123&amp;"_"&amp;G123&amp;"*"</f>
+        <v>R-WH_Det_SOL*</v>
+      </c>
+      <c r="C123" s="32"/>
+      <c r="D123" s="40">
+        <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H123,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>4.6408942067286699E-2</v>
+      </c>
+      <c r="F123" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="G123" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="H123" s="39" t="str">
-        <f t="shared" si="33"/>
-        <v>R-SH_Det_ELC*X1</v>
+      <c r="G123" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="H123" s="32" t="str">
+        <f t="shared" si="28"/>
+        <v>R-WH_Det_SOL*</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="29" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B124" s="30"/>
       <c r="C124" s="31"/>
@@ -8231,16 +8203,13 @@
     </row>
     <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="32" t="s">
-        <v>245</v>
+        <v>78</v>
       </c>
       <c r="B125" s="32" t="str">
-        <f>"R-HC_"&amp;F125&amp;"_"&amp;G125&amp;"_HPN*"</f>
-        <v>R-HC_Apt_ELC_HPN*</v>
-      </c>
-      <c r="C125" s="32" t="str">
-        <f>"RSDSH_"&amp;F125</f>
-        <v>RSDSH_Apt</v>
-      </c>
+        <f>"R-SC_"&amp;F125&amp;"_"&amp;G125&amp;"_N1"</f>
+        <v>R-SC_Apt_ELC_N1</v>
+      </c>
+      <c r="C125" s="32"/>
       <c r="D125" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H125,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>2.6752418704136399E-2</v>
@@ -8251,23 +8220,20 @@
       <c r="G125" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H125" s="32" t="str">
-        <f t="shared" ref="H125:H127" si="34">"R-SH_"&amp;F125&amp;"_"&amp;G125&amp;"*X1"</f>
+      <c r="H125" s="37" t="str">
+        <f t="shared" ref="H125:H127" si="29">"R-SH_"&amp;F125&amp;"_"&amp;G125&amp;"*X1"</f>
         <v>R-SH_Apt_ELC*X1</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="32" t="s">
-        <v>245</v>
+        <v>78</v>
       </c>
       <c r="B126" s="32" t="str">
-        <f>"R-HC_"&amp;F126&amp;"_"&amp;G126&amp;"_HPN*"</f>
-        <v>R-HC_Att_ELC_HPN*</v>
-      </c>
-      <c r="C126" s="32" t="str">
-        <f>"RSDSH_"&amp;F126</f>
-        <v>RSDSH_Att</v>
-      </c>
+        <f>"R-SC_"&amp;F126&amp;"_"&amp;G126&amp;"_N1"</f>
+        <v>R-SC_Att_ELC_N1</v>
+      </c>
+      <c r="C126" s="32"/>
       <c r="D126" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H126,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>2.1795378605209401E-2</v>
@@ -8278,35 +8244,218 @@
       <c r="G126" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H126" s="32" t="str">
-        <f t="shared" si="34"/>
+      <c r="H126" s="37" t="str">
+        <f t="shared" si="29"/>
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="B127" s="38" t="str">
-        <f>"R-HC_"&amp;F127&amp;"_"&amp;G127&amp;"_HPN*"</f>
-        <v>R-HC_Det_ELC_HPN*</v>
-      </c>
-      <c r="C127" s="38" t="str">
-        <f>"RSDSH_"&amp;F127</f>
-        <v>RSDSH_Det</v>
-      </c>
-      <c r="D127" s="38">
+      <c r="A127" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B127" s="32" t="str">
+        <f>"R-SC_"&amp;F127&amp;"_"&amp;G127&amp;"_N1"</f>
+        <v>R-SC_Det_ELC_N1</v>
+      </c>
+      <c r="C127" s="32"/>
+      <c r="D127" s="32">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H127,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
         <v>4.0026061338975703E-2</v>
       </c>
-      <c r="F127" s="38" t="s">
+      <c r="F127" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="G127" s="38" t="s">
+      <c r="G127" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H127" s="38" t="str">
-        <f t="shared" si="34"/>
+      <c r="H127" s="37" t="str">
+        <f t="shared" si="29"/>
+        <v>R-SH_Det_ELC*X1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A128" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="B128" s="30"/>
+      <c r="C128" s="31"/>
+      <c r="D128" s="30"/>
+      <c r="E128" s="30"/>
+      <c r="F128" s="30"/>
+      <c r="G128" s="30"/>
+      <c r="H128" s="30"/>
+    </row>
+    <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B129" s="32" t="str">
+        <f>"R-HC_"&amp;F129&amp;"_"&amp;G129&amp;"_HPN*"</f>
+        <v>R-HC_Apt_ELC_HPN*</v>
+      </c>
+      <c r="C129" s="32" t="str">
+        <f>"RSDSC_"&amp;F129</f>
+        <v>RSDSC_Apt</v>
+      </c>
+      <c r="D129" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H129,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.6752418704136399E-2</v>
+      </c>
+      <c r="F129" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G129" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H129" s="37" t="str">
+        <f t="shared" ref="H129:H131" si="30">"R-SH_"&amp;F129&amp;"_"&amp;G129&amp;"*X1"</f>
+        <v>R-SH_Apt_ELC*X1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B130" s="32" t="str">
+        <f>"R-HC_"&amp;F130&amp;"_"&amp;G130&amp;"_HPN*"</f>
+        <v>R-HC_Att_ELC_HPN*</v>
+      </c>
+      <c r="C130" s="32" t="str">
+        <f>"RSDSC_"&amp;F130</f>
+        <v>RSDSC_Att</v>
+      </c>
+      <c r="D130" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H130,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.1795378605209401E-2</v>
+      </c>
+      <c r="F130" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G130" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H130" s="37" t="str">
+        <f t="shared" si="30"/>
+        <v>R-SH_Att_ELC*X1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="38" t="str">
+        <f>"R-HC_"&amp;F131&amp;"_"&amp;G131&amp;"_HPN*"</f>
+        <v>R-HC_Det_ELC_HPN*</v>
+      </c>
+      <c r="C131" s="38" t="str">
+        <f>"RSDSC_"&amp;F131</f>
+        <v>RSDSC_Det</v>
+      </c>
+      <c r="D131" s="38">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H131,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>4.0026061338975703E-2</v>
+      </c>
+      <c r="F131" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="G131" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="H131" s="39" t="str">
+        <f t="shared" si="30"/>
+        <v>R-SH_Det_ELC*X1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A132" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="B132" s="30"/>
+      <c r="C132" s="31"/>
+      <c r="D132" s="30"/>
+      <c r="E132" s="30"/>
+      <c r="F132" s="30"/>
+      <c r="G132" s="30"/>
+      <c r="H132" s="30"/>
+    </row>
+    <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B133" s="32" t="str">
+        <f>"R-HC_"&amp;F133&amp;"_"&amp;G133&amp;"_HPN*"</f>
+        <v>R-HC_Apt_ELC_HPN*</v>
+      </c>
+      <c r="C133" s="32" t="str">
+        <f>"RSDSH_"&amp;F133</f>
+        <v>RSDSH_Apt</v>
+      </c>
+      <c r="D133" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H133,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.6752418704136399E-2</v>
+      </c>
+      <c r="F133" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G133" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H133" s="32" t="str">
+        <f t="shared" ref="H133:H135" si="31">"R-SH_"&amp;F133&amp;"_"&amp;G133&amp;"*X1"</f>
+        <v>R-SH_Apt_ELC*X1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B134" s="32" t="str">
+        <f>"R-HC_"&amp;F134&amp;"_"&amp;G134&amp;"_HPN*"</f>
+        <v>R-HC_Att_ELC_HPN*</v>
+      </c>
+      <c r="C134" s="32" t="str">
+        <f>"RSDSH_"&amp;F134</f>
+        <v>RSDSH_Att</v>
+      </c>
+      <c r="D134" s="32">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H134,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>2.1795378605209401E-2</v>
+      </c>
+      <c r="F134" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G134" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H134" s="32" t="str">
+        <f t="shared" si="31"/>
+        <v>R-SH_Att_ELC*X1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B135" s="38" t="str">
+        <f>"R-HC_"&amp;F135&amp;"_"&amp;G135&amp;"_HPN*"</f>
+        <v>R-HC_Det_ELC_HPN*</v>
+      </c>
+      <c r="C135" s="38" t="str">
+        <f>"RSDSH_"&amp;F135</f>
+        <v>RSDSH_Det</v>
+      </c>
+      <c r="D135" s="38">
+        <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H135,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
+        <v>4.0026061338975703E-2</v>
+      </c>
+      <c r="F135" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="G135" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="H135" s="38" t="str">
+        <f t="shared" si="31"/>
         <v>R-SH_Det_ELC*X1</v>
       </c>
     </row>
@@ -8324,9 +8473,8 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10253,7 +10401,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11910,9 +12057,6 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="L17" sqref="L17:L18"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13446,7 +13590,6 @@
   <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>